<commit_message>
Atualizado para o dia 20200415
</commit_message>
<xml_diff>
--- a/obj_2020.xlsx
+++ b/obj_2020.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilizador\PycharmProjects\webcomum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B5D9CD1-AEA0-4C24-8338-6286DB945ACB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9E8D9D50-296B-4DF7-99A0-A4124AD6B780}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{782B4511-98CD-3642-962C-2459CDADA9BE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="15000" xr2:uid="{782B4511-98CD-3642-962C-2459CDADA9BE}"/>
   </bookViews>
   <sheets>
     <sheet name="2020" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <definedName name="_FilterDatabase" localSheetId="3" hidden="1">árvore!$A$1:$C$1</definedName>
     <definedName name="_FilterDatabase" localSheetId="2" hidden="1">'CNP Planograma'!$A$1:$E$1</definedName>
     <definedName name="_FilterDatabase" localSheetId="4" hidden="1">inverno!$A$1:$G$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2020'!$A$1:$G$331</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3768" uniqueCount="826">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3596" uniqueCount="838">
   <si>
     <t>Categoria hmR3</t>
   </si>
@@ -2352,15 +2353,9 @@
     <t>Lactacyd Medicinal</t>
   </si>
   <si>
-    <t>6323048</t>
-  </si>
-  <si>
     <t xml:space="preserve">ValdispertNoite Rapid + x 20 comp orodisp (substitui o Rapid </t>
   </si>
   <si>
-    <t>6384727</t>
-  </si>
-  <si>
     <t>Valdispert Noite &amp; Dia Comp X20+20</t>
   </si>
   <si>
@@ -2409,9 +2404,6 @@
     <t>Prostamol</t>
   </si>
   <si>
-    <t>7473355</t>
-  </si>
-  <si>
     <t>Prostamol caps</t>
   </si>
   <si>
@@ -2490,16 +2482,10 @@
     <t>Hepatoprotetor em solução oral hmR 4</t>
   </si>
   <si>
-    <t>Prevenção e alívio das dores/lesões pelo calor emplastro hmR 4</t>
-  </si>
-  <si>
     <t>Tratamento e cuidado de pernas pesadas sistémico hmR 4</t>
   </si>
   <si>
     <t>Anti-inflamatórios e Anti-Reumáticos tópicos emplastro hmR 4</t>
-  </si>
-  <si>
-    <t>Enemas solução retal hmR 4</t>
   </si>
   <si>
     <t>Reguladores da flora intestinal pó hmR 4</t>
@@ -2584,6 +2570,57 @@
       </rPr>
       <t xml:space="preserve"> hmR 4</t>
     </r>
+  </si>
+  <si>
+    <t>Prevenção e alívio das dores/lesões pelo calor emplastro hmR 5</t>
+  </si>
+  <si>
+    <t>Enemas solução retal hmR 5</t>
+  </si>
+  <si>
+    <t>NeoBianacid</t>
+  </si>
+  <si>
+    <t>Voltaren - GSK</t>
+  </si>
+  <si>
+    <t>VitaCê</t>
+  </si>
+  <si>
+    <t>FullMarks</t>
+  </si>
+  <si>
+    <t>Sperti Preparacao H</t>
+  </si>
+  <si>
+    <t>Neo-Sinefrina</t>
+  </si>
+  <si>
+    <t>VoltaTermic</t>
+  </si>
+  <si>
+    <t>ThermaCare</t>
+  </si>
+  <si>
+    <t>Procto-Glyvenol</t>
+  </si>
+  <si>
+    <t>Aloclair Plus</t>
+  </si>
+  <si>
+    <t>Aquilea</t>
+  </si>
+  <si>
+    <t>Viv Nutri</t>
+  </si>
+  <si>
+    <t>Symbiosys</t>
+  </si>
+  <si>
+    <t>Fitoroid</t>
+  </si>
+  <si>
+    <t>Pedisilk</t>
   </si>
 </sst>
 </file>
@@ -3764,8 +3801,8 @@
   </sheetPr>
   <dimension ref="A1:K331"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J2" sqref="J1:K1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="14.25"/>
@@ -3875,6 +3912,7 @@
       <c r="G4" s="85">
         <v>0.8</v>
       </c>
+      <c r="I4" s="26"/>
       <c r="K4" s="26"/>
     </row>
     <row r="5" spans="1:11" ht="15.95" customHeight="1">
@@ -4031,8 +4069,8 @@
       <c r="C11" s="60" t="s">
         <v>490</v>
       </c>
-      <c r="D11" s="29" t="s">
-        <v>491</v>
+      <c r="D11" s="29">
+        <v>6597344</v>
       </c>
       <c r="E11" s="67" t="s">
         <v>492</v>
@@ -4317,7 +4355,7 @@
         <v>13</v>
       </c>
       <c r="C23" s="60" t="s">
-        <v>50</v>
+        <v>823</v>
       </c>
       <c r="D23" s="28">
         <v>6226506</v>
@@ -4341,7 +4379,7 @@
         <v>13</v>
       </c>
       <c r="C24" s="60" t="s">
-        <v>50</v>
+        <v>823</v>
       </c>
       <c r="D24" s="28">
         <v>6406413</v>
@@ -4367,8 +4405,8 @@
       <c r="C25" s="60" t="s">
         <v>39</v>
       </c>
-      <c r="D25" s="28" t="s">
-        <v>40</v>
+      <c r="D25" s="28">
+        <v>5281407</v>
       </c>
       <c r="E25" s="66" t="s">
         <v>41</v>
@@ -4391,8 +4429,8 @@
       <c r="C26" s="65" t="s">
         <v>39</v>
       </c>
-      <c r="D26" s="28" t="s">
-        <v>42</v>
+      <c r="D26" s="28">
+        <v>5606256</v>
       </c>
       <c r="E26" s="66" t="s">
         <v>43</v>
@@ -4415,8 +4453,8 @@
       <c r="C27" s="65" t="s">
         <v>39</v>
       </c>
-      <c r="D27" s="28" t="s">
-        <v>44</v>
+      <c r="D27" s="28">
+        <v>5281431</v>
       </c>
       <c r="E27" s="66" t="s">
         <v>45</v>
@@ -4439,8 +4477,8 @@
       <c r="C28" s="65" t="s">
         <v>39</v>
       </c>
-      <c r="D28" s="28" t="s">
-        <v>46</v>
+      <c r="D28" s="28">
+        <v>5490925</v>
       </c>
       <c r="E28" s="66" t="s">
         <v>47</v>
@@ -4463,8 +4501,8 @@
       <c r="C29" s="60" t="s">
         <v>39</v>
       </c>
-      <c r="D29" s="28" t="s">
-        <v>48</v>
+      <c r="D29" s="28">
+        <v>5630355</v>
       </c>
       <c r="E29" s="66" t="s">
         <v>49</v>
@@ -4487,8 +4525,8 @@
       <c r="C30" s="65" t="s">
         <v>59</v>
       </c>
-      <c r="D30" s="28" t="s">
-        <v>60</v>
+      <c r="D30" s="28">
+        <v>5335955</v>
       </c>
       <c r="E30" s="66" t="s">
         <v>61</v>
@@ -4511,8 +4549,8 @@
       <c r="C31" s="65" t="s">
         <v>59</v>
       </c>
-      <c r="D31" s="28" t="s">
-        <v>62</v>
+      <c r="D31" s="28">
+        <v>8434902</v>
       </c>
       <c r="E31" s="66" t="s">
         <v>63</v>
@@ -4599,7 +4637,7 @@
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="72" t="s">
-        <v>801</v>
+        <v>798</v>
       </c>
       <c r="B35" s="22" t="s">
         <v>396</v>
@@ -4611,7 +4649,7 @@
         <v>5658323</v>
       </c>
       <c r="E35" s="66" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="F35" s="83">
         <v>0.25</v>
@@ -4623,7 +4661,7 @@
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="72" t="s">
-        <v>801</v>
+        <v>798</v>
       </c>
       <c r="B36" s="22" t="s">
         <v>33</v>
@@ -4635,7 +4673,7 @@
         <v>0</v>
       </c>
       <c r="E36" s="66" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="F36" s="83">
         <v>0.08</v>
@@ -4647,7 +4685,7 @@
     </row>
     <row r="37" spans="1:10">
       <c r="A37" s="72" t="s">
-        <v>800</v>
+        <v>797</v>
       </c>
       <c r="B37" s="22" t="s">
         <v>33</v>
@@ -4671,7 +4709,7 @@
     </row>
     <row r="38" spans="1:10">
       <c r="A38" s="72" t="s">
-        <v>799</v>
+        <v>796</v>
       </c>
       <c r="B38" s="22" t="s">
         <v>28</v>
@@ -4695,7 +4733,7 @@
     </row>
     <row r="39" spans="1:10">
       <c r="A39" s="72" t="s">
-        <v>802</v>
+        <v>799</v>
       </c>
       <c r="B39" s="38" t="s">
         <v>73</v>
@@ -4703,8 +4741,8 @@
       <c r="C39" s="61" t="s">
         <v>74</v>
       </c>
-      <c r="D39" s="29" t="s">
-        <v>75</v>
+      <c r="D39" s="29">
+        <v>8912410</v>
       </c>
       <c r="E39" s="67" t="s">
         <v>76</v>
@@ -4719,7 +4757,7 @@
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="72" t="s">
-        <v>802</v>
+        <v>799</v>
       </c>
       <c r="B40" s="22" t="s">
         <v>77</v>
@@ -4743,7 +4781,7 @@
     </row>
     <row r="41" spans="1:10">
       <c r="A41" s="72" t="s">
-        <v>802</v>
+        <v>799</v>
       </c>
       <c r="B41" s="22" t="s">
         <v>77</v>
@@ -4775,8 +4813,8 @@
       <c r="C42" s="64" t="s">
         <v>82</v>
       </c>
-      <c r="D42" s="29" t="s">
-        <v>83</v>
+      <c r="D42" s="29">
+        <v>6966093</v>
       </c>
       <c r="E42" s="119" t="s">
         <v>84</v>
@@ -4799,8 +4837,8 @@
       <c r="C43" s="64" t="s">
         <v>82</v>
       </c>
-      <c r="D43" s="29" t="s">
-        <v>85</v>
+      <c r="D43" s="29">
+        <v>7004895</v>
       </c>
       <c r="E43" s="119" t="s">
         <v>86</v>
@@ -4823,8 +4861,8 @@
       <c r="C44" s="60" t="s">
         <v>82</v>
       </c>
-      <c r="D44" s="29" t="s">
-        <v>87</v>
+      <c r="D44" s="29">
+        <v>6952333</v>
       </c>
       <c r="E44" s="119" t="s">
         <v>88</v>
@@ -4869,10 +4907,10 @@
         <v>8</v>
       </c>
       <c r="C46" s="60" t="s">
-        <v>142</v>
-      </c>
-      <c r="D46" s="29" t="s">
-        <v>143</v>
+        <v>837</v>
+      </c>
+      <c r="D46" s="29">
+        <v>6004424</v>
       </c>
       <c r="E46" s="67" t="s">
         <v>144</v>
@@ -4895,8 +4933,8 @@
       <c r="C47" s="60" t="s">
         <v>145</v>
       </c>
-      <c r="D47" s="29" t="s">
-        <v>146</v>
+      <c r="D47" s="29">
+        <v>5743521</v>
       </c>
       <c r="E47" s="67" t="s">
         <v>147</v>
@@ -4919,8 +4957,8 @@
       <c r="C48" s="60" t="s">
         <v>145</v>
       </c>
-      <c r="D48" s="29" t="s">
-        <v>148</v>
+      <c r="D48" s="29">
+        <v>6872184</v>
       </c>
       <c r="E48" s="67" t="s">
         <v>149</v>
@@ -4943,8 +4981,8 @@
       <c r="C49" s="76" t="s">
         <v>130</v>
       </c>
-      <c r="D49" s="29" t="s">
-        <v>133</v>
+      <c r="D49" s="29">
+        <v>6316679</v>
       </c>
       <c r="E49" s="67" t="s">
         <v>134</v>
@@ -4967,8 +5005,8 @@
       <c r="C50" s="76" t="s">
         <v>130</v>
       </c>
-      <c r="D50" s="29" t="s">
-        <v>135</v>
+      <c r="D50" s="29">
+        <v>6316661</v>
       </c>
       <c r="E50" s="67" t="s">
         <v>136</v>
@@ -4991,8 +5029,8 @@
       <c r="C51" s="76" t="s">
         <v>130</v>
       </c>
-      <c r="D51" s="29" t="s">
-        <v>137</v>
+      <c r="D51" s="29">
+        <v>6087791</v>
       </c>
       <c r="E51" s="67" t="s">
         <v>138</v>
@@ -5007,7 +5045,7 @@
     </row>
     <row r="52" spans="1:10" ht="15.95" customHeight="1">
       <c r="A52" s="79" t="s">
-        <v>805</v>
+        <v>802</v>
       </c>
       <c r="B52" s="22" t="s">
         <v>28</v>
@@ -5031,7 +5069,7 @@
     </row>
     <row r="53" spans="1:10">
       <c r="A53" s="72" t="s">
-        <v>805</v>
+        <v>802</v>
       </c>
       <c r="B53" s="22" t="s">
         <v>153</v>
@@ -5055,7 +5093,7 @@
     </row>
     <row r="54" spans="1:10" ht="15.95" customHeight="1">
       <c r="A54" s="72" t="s">
-        <v>805</v>
+        <v>802</v>
       </c>
       <c r="B54" s="22" t="s">
         <v>8</v>
@@ -5079,7 +5117,7 @@
     </row>
     <row r="55" spans="1:10" ht="15.95" customHeight="1">
       <c r="A55" s="72" t="s">
-        <v>806</v>
+        <v>803</v>
       </c>
       <c r="B55" s="22" t="s">
         <v>153</v>
@@ -5103,7 +5141,7 @@
     </row>
     <row r="56" spans="1:10">
       <c r="A56" s="72" t="s">
-        <v>807</v>
+        <v>804</v>
       </c>
       <c r="B56" s="22" t="s">
         <v>8</v>
@@ -5127,7 +5165,7 @@
     </row>
     <row r="57" spans="1:10" ht="15.95" customHeight="1">
       <c r="A57" s="72" t="s">
-        <v>807</v>
+        <v>804</v>
       </c>
       <c r="B57" s="22" t="s">
         <v>161</v>
@@ -5151,13 +5189,13 @@
     </row>
     <row r="58" spans="1:10" ht="15.95" customHeight="1">
       <c r="A58" s="72" t="s">
-        <v>803</v>
+        <v>800</v>
       </c>
       <c r="B58" s="22" t="s">
         <v>90</v>
       </c>
       <c r="C58" s="65" t="s">
-        <v>91</v>
+        <v>831</v>
       </c>
       <c r="D58" s="28">
         <v>5337498</v>
@@ -5175,13 +5213,13 @@
     </row>
     <row r="59" spans="1:10" ht="15.95" customHeight="1">
       <c r="A59" s="72" t="s">
-        <v>803</v>
+        <v>800</v>
       </c>
       <c r="B59" s="22" t="s">
         <v>732</v>
       </c>
       <c r="C59" s="65" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="D59" s="28">
         <v>9658914</v>
@@ -5199,16 +5237,16 @@
     </row>
     <row r="60" spans="1:10" ht="15.95" customHeight="1">
       <c r="A60" s="72" t="s">
-        <v>803</v>
+        <v>800</v>
       </c>
       <c r="B60" s="22" t="s">
         <v>55</v>
       </c>
       <c r="C60" s="65" t="s">
-        <v>93</v>
-      </c>
-      <c r="D60" s="28" t="s">
-        <v>96</v>
+        <v>827</v>
+      </c>
+      <c r="D60" s="28">
+        <v>8573014</v>
       </c>
       <c r="E60" s="66" t="s">
         <v>97</v>
@@ -5223,13 +5261,13 @@
     </row>
     <row r="61" spans="1:10" ht="15.95" customHeight="1">
       <c r="A61" s="72" t="s">
-        <v>803</v>
+        <v>800</v>
       </c>
       <c r="B61" s="22" t="s">
         <v>13</v>
       </c>
       <c r="C61" s="65" t="s">
-        <v>98</v>
+        <v>836</v>
       </c>
       <c r="D61" s="28">
         <v>6968438</v>
@@ -5247,19 +5285,19 @@
     </row>
     <row r="62" spans="1:10" ht="15.95" customHeight="1">
       <c r="A62" s="72" t="s">
-        <v>804</v>
+        <v>801</v>
       </c>
       <c r="B62" s="22" t="s">
         <v>732</v>
       </c>
       <c r="C62" s="65" t="s">
-        <v>777</v>
+        <v>731</v>
       </c>
       <c r="D62" s="28">
         <v>9579003</v>
       </c>
       <c r="E62" s="66" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="F62" s="77">
         <v>0.7</v>
@@ -5271,16 +5309,16 @@
     </row>
     <row r="63" spans="1:10" ht="15.95" customHeight="1">
       <c r="A63" s="72" t="s">
-        <v>804</v>
+        <v>801</v>
       </c>
       <c r="B63" s="22" t="s">
         <v>55</v>
       </c>
       <c r="C63" s="65" t="s">
-        <v>93</v>
-      </c>
-      <c r="D63" s="28" t="s">
-        <v>94</v>
+        <v>827</v>
+      </c>
+      <c r="D63" s="28">
+        <v>8289611</v>
       </c>
       <c r="E63" s="66" t="s">
         <v>95</v>
@@ -5295,7 +5333,7 @@
     </row>
     <row r="64" spans="1:10" ht="15.95" customHeight="1">
       <c r="A64" s="72" t="s">
-        <v>810</v>
+        <v>807</v>
       </c>
       <c r="B64" s="22" t="s">
         <v>28</v>
@@ -5319,7 +5357,7 @@
     </row>
     <row r="65" spans="1:10" ht="15.95" customHeight="1">
       <c r="A65" s="72" t="s">
-        <v>810</v>
+        <v>807</v>
       </c>
       <c r="B65" s="22" t="s">
         <v>28</v>
@@ -5343,7 +5381,7 @@
     </row>
     <row r="66" spans="1:10" ht="15.95" customHeight="1">
       <c r="A66" s="72" t="s">
-        <v>810</v>
+        <v>807</v>
       </c>
       <c r="B66" s="22" t="s">
         <v>33</v>
@@ -5367,7 +5405,7 @@
     </row>
     <row r="67" spans="1:10" ht="15.95" customHeight="1">
       <c r="A67" s="72" t="s">
-        <v>810</v>
+        <v>807</v>
       </c>
       <c r="B67" s="22" t="s">
         <v>24</v>
@@ -5391,7 +5429,7 @@
     </row>
     <row r="68" spans="1:10" ht="15.95" customHeight="1">
       <c r="A68" s="72" t="s">
-        <v>810</v>
+        <v>807</v>
       </c>
       <c r="B68" s="22" t="s">
         <v>24</v>
@@ -5415,7 +5453,7 @@
     </row>
     <row r="69" spans="1:10" ht="15.95" customHeight="1">
       <c r="A69" s="72" t="s">
-        <v>810</v>
+        <v>807</v>
       </c>
       <c r="B69" s="22" t="s">
         <v>24</v>
@@ -5439,7 +5477,7 @@
     </row>
     <row r="70" spans="1:10" ht="15.95" customHeight="1">
       <c r="A70" s="72" t="s">
-        <v>810</v>
+        <v>807</v>
       </c>
       <c r="B70" s="22" t="s">
         <v>24</v>
@@ -5463,7 +5501,7 @@
     </row>
     <row r="71" spans="1:10" ht="15.95" customHeight="1">
       <c r="A71" s="80" t="s">
-        <v>817</v>
+        <v>813</v>
       </c>
       <c r="B71" s="22" t="s">
         <v>28</v>
@@ -5487,7 +5525,7 @@
     </row>
     <row r="72" spans="1:10">
       <c r="A72" s="80" t="s">
-        <v>817</v>
+        <v>813</v>
       </c>
       <c r="B72" s="38" t="s">
         <v>139</v>
@@ -5511,7 +5549,7 @@
     </row>
     <row r="73" spans="1:10" ht="15.95" customHeight="1">
       <c r="A73" s="80" t="s">
-        <v>823</v>
+        <v>818</v>
       </c>
       <c r="B73" s="22" t="s">
         <v>749</v>
@@ -5535,7 +5573,7 @@
     </row>
     <row r="74" spans="1:10" ht="15">
       <c r="A74" s="80" t="s">
-        <v>823</v>
+        <v>818</v>
       </c>
       <c r="B74" s="38" t="s">
         <v>749</v>
@@ -5559,7 +5597,7 @@
     </row>
     <row r="75" spans="1:10" ht="15.95" customHeight="1">
       <c r="A75" s="138" t="s">
-        <v>823</v>
+        <v>818</v>
       </c>
       <c r="B75" s="32" t="s">
         <v>749</v>
@@ -5583,7 +5621,7 @@
     </row>
     <row r="76" spans="1:10" ht="15.95" customHeight="1">
       <c r="A76" s="138" t="s">
-        <v>823</v>
+        <v>818</v>
       </c>
       <c r="B76" s="22" t="s">
         <v>749</v>
@@ -5607,7 +5645,7 @@
     </row>
     <row r="77" spans="1:10" ht="15.95" customHeight="1">
       <c r="A77" s="80" t="s">
-        <v>823</v>
+        <v>818</v>
       </c>
       <c r="B77" s="22" t="s">
         <v>749</v>
@@ -5631,7 +5669,7 @@
     </row>
     <row r="78" spans="1:10" ht="15">
       <c r="A78" s="80" t="s">
-        <v>823</v>
+        <v>818</v>
       </c>
       <c r="B78" s="38" t="s">
         <v>749</v>
@@ -5655,13 +5693,13 @@
     </row>
     <row r="79" spans="1:10" ht="15.95" customHeight="1">
       <c r="A79" s="80" t="s">
-        <v>823</v>
+        <v>818</v>
       </c>
       <c r="B79" s="22" t="s">
         <v>28</v>
       </c>
       <c r="C79" s="60" t="s">
-        <v>362</v>
+        <v>824</v>
       </c>
       <c r="D79" s="28">
         <v>5197868</v>
@@ -5679,13 +5717,13 @@
     </row>
     <row r="80" spans="1:10" ht="15.95" customHeight="1">
       <c r="A80" s="80" t="s">
-        <v>823</v>
+        <v>818</v>
       </c>
       <c r="B80" s="22" t="s">
         <v>28</v>
       </c>
       <c r="C80" s="60" t="s">
-        <v>362</v>
+        <v>824</v>
       </c>
       <c r="D80" s="28">
         <v>5035654</v>
@@ -5703,13 +5741,13 @@
     </row>
     <row r="81" spans="1:10" ht="15">
       <c r="A81" s="80" t="s">
-        <v>823</v>
+        <v>818</v>
       </c>
       <c r="B81" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="C81" s="61" t="s">
-        <v>362</v>
+      <c r="C81" s="60" t="s">
+        <v>824</v>
       </c>
       <c r="D81" s="28">
         <v>5712740</v>
@@ -5727,13 +5765,13 @@
     </row>
     <row r="82" spans="1:10" ht="15">
       <c r="A82" s="80" t="s">
-        <v>823</v>
+        <v>818</v>
       </c>
       <c r="B82" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C82" s="65" t="s">
-        <v>362</v>
+      <c r="C82" s="60" t="s">
+        <v>824</v>
       </c>
       <c r="D82" s="28">
         <v>5219316</v>
@@ -5751,13 +5789,13 @@
     </row>
     <row r="83" spans="1:10" ht="15">
       <c r="A83" s="80" t="s">
-        <v>823</v>
+        <v>818</v>
       </c>
       <c r="B83" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C83" s="123" t="s">
-        <v>359</v>
+      <c r="C83" s="60" t="s">
+        <v>824</v>
       </c>
       <c r="D83" s="154">
         <v>5374848</v>
@@ -5775,13 +5813,13 @@
     </row>
     <row r="84" spans="1:10" ht="15">
       <c r="A84" s="80" t="s">
-        <v>823</v>
+        <v>818</v>
       </c>
       <c r="B84" s="22" t="s">
         <v>28</v>
       </c>
       <c r="C84" s="60" t="s">
-        <v>359</v>
+        <v>824</v>
       </c>
       <c r="D84" s="28">
         <v>5625025</v>
@@ -5799,13 +5837,13 @@
     </row>
     <row r="85" spans="1:10" ht="15">
       <c r="A85" s="80" t="s">
-        <v>823</v>
+        <v>818</v>
       </c>
       <c r="B85" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C85" s="101" t="s">
-        <v>359</v>
+      <c r="C85" s="60" t="s">
+        <v>824</v>
       </c>
       <c r="D85" s="102">
         <v>5380571</v>
@@ -5831,8 +5869,8 @@
       <c r="C86" s="60" t="s">
         <v>101</v>
       </c>
-      <c r="D86" s="78" t="s">
-        <v>102</v>
+      <c r="D86" s="78">
+        <v>6840637</v>
       </c>
       <c r="E86" s="67" t="s">
         <v>103</v>
@@ -5855,8 +5893,8 @@
       <c r="C87" s="60" t="s">
         <v>101</v>
       </c>
-      <c r="D87" s="29" t="s">
-        <v>104</v>
+      <c r="D87" s="29">
+        <v>6201038</v>
       </c>
       <c r="E87" s="67" t="s">
         <v>105</v>
@@ -5879,8 +5917,8 @@
       <c r="C88" s="60" t="s">
         <v>101</v>
       </c>
-      <c r="D88" s="29" t="s">
-        <v>106</v>
+      <c r="D88" s="29">
+        <v>6186452</v>
       </c>
       <c r="E88" s="67" t="s">
         <v>107</v>
@@ -5903,8 +5941,8 @@
       <c r="C89" s="60" t="s">
         <v>101</v>
       </c>
-      <c r="D89" s="29" t="s">
-        <v>108</v>
+      <c r="D89" s="29">
+        <v>7759217</v>
       </c>
       <c r="E89" s="67" t="s">
         <v>109</v>
@@ -5927,8 +5965,8 @@
       <c r="C90" s="60" t="s">
         <v>101</v>
       </c>
-      <c r="D90" s="29" t="s">
-        <v>110</v>
+      <c r="D90" s="29">
+        <v>7759209</v>
       </c>
       <c r="E90" s="67" t="s">
         <v>111</v>
@@ -5951,8 +5989,8 @@
       <c r="C91" s="60" t="s">
         <v>101</v>
       </c>
-      <c r="D91" s="29" t="s">
-        <v>113</v>
+      <c r="D91" s="29">
+        <v>6089060</v>
       </c>
       <c r="E91" s="67" t="s">
         <v>114</v>
@@ -5975,8 +6013,8 @@
       <c r="C92" s="60" t="s">
         <v>101</v>
       </c>
-      <c r="D92" s="29" t="s">
-        <v>115</v>
+      <c r="D92" s="29">
+        <v>6287573</v>
       </c>
       <c r="E92" s="67" t="s">
         <v>116</v>
@@ -5997,10 +6035,10 @@
         <v>24</v>
       </c>
       <c r="C93" s="60" t="s">
-        <v>112</v>
-      </c>
-      <c r="D93" s="29" t="s">
-        <v>117</v>
+        <v>826</v>
+      </c>
+      <c r="D93" s="29">
+        <v>6317586</v>
       </c>
       <c r="E93" s="67" t="s">
         <v>118</v>
@@ -6021,10 +6059,10 @@
         <v>24</v>
       </c>
       <c r="C94" s="60" t="s">
-        <v>112</v>
-      </c>
-      <c r="D94" s="29" t="s">
-        <v>119</v>
+        <v>826</v>
+      </c>
+      <c r="D94" s="29">
+        <v>6942466</v>
       </c>
       <c r="E94" s="67" t="s">
         <v>120</v>
@@ -6045,10 +6083,10 @@
         <v>24</v>
       </c>
       <c r="C95" s="60" t="s">
-        <v>112</v>
-      </c>
-      <c r="D95" s="29" t="s">
-        <v>121</v>
+        <v>826</v>
+      </c>
+      <c r="D95" s="29">
+        <v>7008029</v>
       </c>
       <c r="E95" s="67" t="s">
         <v>122</v>
@@ -6069,10 +6107,10 @@
         <v>24</v>
       </c>
       <c r="C96" s="60" t="s">
-        <v>112</v>
-      </c>
-      <c r="D96" s="29" t="s">
-        <v>123</v>
+        <v>826</v>
+      </c>
+      <c r="D96" s="29">
+        <v>6992040</v>
       </c>
       <c r="E96" s="67" t="s">
         <v>124</v>
@@ -6093,10 +6131,10 @@
         <v>24</v>
       </c>
       <c r="C97" s="60" t="s">
-        <v>112</v>
-      </c>
-      <c r="D97" s="29" t="s">
-        <v>125</v>
+        <v>826</v>
+      </c>
+      <c r="D97" s="29">
+        <v>7471698</v>
       </c>
       <c r="E97" s="67" t="s">
         <v>126</v>
@@ -6117,10 +6155,10 @@
         <v>24</v>
       </c>
       <c r="C98" s="60" t="s">
-        <v>112</v>
-      </c>
-      <c r="D98" s="29" t="s">
-        <v>127</v>
+        <v>826</v>
+      </c>
+      <c r="D98" s="29">
+        <v>6076588</v>
       </c>
       <c r="E98" s="67" t="s">
         <v>128</v>
@@ -6311,8 +6349,8 @@
       <c r="C106" s="76" t="s">
         <v>177</v>
       </c>
-      <c r="D106" s="29" t="s">
-        <v>178</v>
+      <c r="D106" s="29">
+        <v>7954719</v>
       </c>
       <c r="E106" s="67" t="s">
         <v>179</v>
@@ -6335,8 +6373,8 @@
       <c r="C107" s="76" t="s">
         <v>177</v>
       </c>
-      <c r="D107" s="29" t="s">
-        <v>180</v>
+      <c r="D107" s="29">
+        <v>6933465</v>
       </c>
       <c r="E107" s="67" t="s">
         <v>181</v>
@@ -6359,8 +6397,8 @@
       <c r="C108" s="76" t="s">
         <v>177</v>
       </c>
-      <c r="D108" s="29" t="s">
-        <v>182</v>
+      <c r="D108" s="29">
+        <v>6933457</v>
       </c>
       <c r="E108" s="67" t="s">
         <v>183</v>
@@ -6383,8 +6421,8 @@
       <c r="C109" s="76" t="s">
         <v>177</v>
       </c>
-      <c r="D109" s="29" t="s">
-        <v>184</v>
+      <c r="D109" s="29">
+        <v>6057471</v>
       </c>
       <c r="E109" s="67" t="s">
         <v>185</v>
@@ -6407,8 +6445,8 @@
       <c r="C110" s="76" t="s">
         <v>177</v>
       </c>
-      <c r="D110" s="29" t="s">
-        <v>186</v>
+      <c r="D110" s="29">
+        <v>6277830</v>
       </c>
       <c r="E110" s="67" t="s">
         <v>187</v>
@@ -6431,8 +6469,8 @@
       <c r="C111" s="76" t="s">
         <v>188</v>
       </c>
-      <c r="D111" s="29" t="s">
-        <v>189</v>
+      <c r="D111" s="29">
+        <v>6011635</v>
       </c>
       <c r="E111" s="67" t="s">
         <v>190</v>
@@ -6455,8 +6493,8 @@
       <c r="C112" s="76" t="s">
         <v>188</v>
       </c>
-      <c r="D112" s="29" t="s">
-        <v>191</v>
+      <c r="D112" s="29">
+        <v>6166868</v>
       </c>
       <c r="E112" s="67" t="s">
         <v>192</v>
@@ -6479,8 +6517,8 @@
       <c r="C113" s="76" t="s">
         <v>188</v>
       </c>
-      <c r="D113" s="29" t="s">
-        <v>193</v>
+      <c r="D113" s="29">
+        <v>6180547</v>
       </c>
       <c r="E113" s="67" t="s">
         <v>194</v>
@@ -6503,8 +6541,8 @@
       <c r="C114" s="76" t="s">
         <v>188</v>
       </c>
-      <c r="D114" s="29" t="s">
-        <v>195</v>
+      <c r="D114" s="29">
+        <v>6966358</v>
       </c>
       <c r="E114" s="67" t="s">
         <v>196</v>
@@ -6527,8 +6565,8 @@
       <c r="C115" s="76" t="s">
         <v>188</v>
       </c>
-      <c r="D115" s="29" t="s">
-        <v>197</v>
+      <c r="D115" s="29">
+        <v>6550814</v>
       </c>
       <c r="E115" s="67" t="s">
         <v>198</v>
@@ -6551,8 +6589,8 @@
       <c r="C116" s="76" t="s">
         <v>188</v>
       </c>
-      <c r="D116" s="29" t="s">
-        <v>199</v>
+      <c r="D116" s="29">
+        <v>6418103</v>
       </c>
       <c r="E116" s="67" t="s">
         <v>200</v>
@@ -6575,8 +6613,8 @@
       <c r="C117" s="76" t="s">
         <v>188</v>
       </c>
-      <c r="D117" s="29" t="s">
-        <v>201</v>
+      <c r="D117" s="29">
+        <v>6020933</v>
       </c>
       <c r="E117" s="67" t="s">
         <v>202</v>
@@ -6599,8 +6637,8 @@
       <c r="C118" s="76" t="s">
         <v>188</v>
       </c>
-      <c r="D118" s="29" t="s">
-        <v>203</v>
+      <c r="D118" s="29">
+        <v>6299248</v>
       </c>
       <c r="E118" s="67" t="s">
         <v>204</v>
@@ -6623,8 +6661,8 @@
       <c r="C119" s="76" t="s">
         <v>188</v>
       </c>
-      <c r="D119" s="29" t="s">
-        <v>205</v>
+      <c r="D119" s="29">
+        <v>6213819</v>
       </c>
       <c r="E119" s="67" t="s">
         <v>206</v>
@@ -6647,8 +6685,8 @@
       <c r="C120" s="76" t="s">
         <v>188</v>
       </c>
-      <c r="D120" s="29" t="s">
-        <v>207</v>
+      <c r="D120" s="29">
+        <v>6811901</v>
       </c>
       <c r="E120" s="67" t="s">
         <v>208</v>
@@ -6670,8 +6708,8 @@
       <c r="C121" s="76" t="s">
         <v>188</v>
       </c>
-      <c r="D121" s="29" t="s">
-        <v>209</v>
+      <c r="D121" s="29">
+        <v>7475798</v>
       </c>
       <c r="E121" s="67" t="s">
         <v>210</v>
@@ -6693,8 +6731,8 @@
       <c r="C122" s="76" t="s">
         <v>188</v>
       </c>
-      <c r="D122" s="29" t="s">
-        <v>211</v>
+      <c r="D122" s="29">
+        <v>7508838</v>
       </c>
       <c r="E122" s="67" t="s">
         <v>212</v>
@@ -6716,8 +6754,8 @@
       <c r="C123" s="76" t="s">
         <v>188</v>
       </c>
-      <c r="D123" s="29" t="s">
-        <v>213</v>
+      <c r="D123" s="29">
+        <v>6228338</v>
       </c>
       <c r="E123" s="67" t="s">
         <v>214</v>
@@ -6739,8 +6777,8 @@
       <c r="C124" s="60" t="s">
         <v>216</v>
       </c>
-      <c r="D124" s="29" t="s">
-        <v>217</v>
+      <c r="D124" s="29">
+        <v>6593772</v>
       </c>
       <c r="E124" s="67" t="s">
         <v>218</v>
@@ -6762,8 +6800,8 @@
       <c r="C125" s="60" t="s">
         <v>216</v>
       </c>
-      <c r="D125" s="29" t="s">
-        <v>219</v>
+      <c r="D125" s="29">
+        <v>6784108</v>
       </c>
       <c r="E125" s="67" t="s">
         <v>220</v>
@@ -6785,8 +6823,8 @@
       <c r="C126" s="60" t="s">
         <v>216</v>
       </c>
-      <c r="D126" s="29" t="s">
-        <v>221</v>
+      <c r="D126" s="29">
+        <v>6784116</v>
       </c>
       <c r="E126" s="67" t="s">
         <v>222</v>
@@ -6808,8 +6846,8 @@
       <c r="C127" s="60" t="s">
         <v>216</v>
       </c>
-      <c r="D127" s="29" t="s">
-        <v>223</v>
+      <c r="D127" s="29">
+        <v>6405878</v>
       </c>
       <c r="E127" s="67" t="s">
         <v>224</v>
@@ -6831,8 +6869,8 @@
       <c r="C128" s="60" t="s">
         <v>216</v>
       </c>
-      <c r="D128" s="29" t="s">
-        <v>225</v>
+      <c r="D128" s="29">
+        <v>6887182</v>
       </c>
       <c r="E128" s="67" t="s">
         <v>226</v>
@@ -6854,8 +6892,8 @@
       <c r="C129" s="60" t="s">
         <v>216</v>
       </c>
-      <c r="D129" s="29" t="s">
-        <v>227</v>
+      <c r="D129" s="29">
+        <v>6887208</v>
       </c>
       <c r="E129" s="67" t="s">
         <v>228</v>
@@ -6877,8 +6915,8 @@
       <c r="C130" s="60" t="s">
         <v>216</v>
       </c>
-      <c r="D130" s="29" t="s">
-        <v>229</v>
+      <c r="D130" s="29">
+        <v>6985895</v>
       </c>
       <c r="E130" s="67" t="s">
         <v>230</v>
@@ -6900,8 +6938,8 @@
       <c r="C131" s="60" t="s">
         <v>216</v>
       </c>
-      <c r="D131" s="29" t="s">
-        <v>231</v>
+      <c r="D131" s="29">
+        <v>6887893</v>
       </c>
       <c r="E131" s="67" t="s">
         <v>232</v>
@@ -6923,8 +6961,8 @@
       <c r="C132" s="60" t="s">
         <v>216</v>
       </c>
-      <c r="D132" s="29" t="s">
-        <v>233</v>
+      <c r="D132" s="29">
+        <v>6887190</v>
       </c>
       <c r="E132" s="67" t="s">
         <v>234</v>
@@ -6946,8 +6984,8 @@
       <c r="C133" s="60" t="s">
         <v>216</v>
       </c>
-      <c r="D133" s="29" t="s">
-        <v>235</v>
+      <c r="D133" s="29">
+        <v>6887174</v>
       </c>
       <c r="E133" s="67" t="s">
         <v>236</v>
@@ -6969,8 +7007,8 @@
       <c r="C134" s="60" t="s">
         <v>216</v>
       </c>
-      <c r="D134" s="29" t="s">
-        <v>237</v>
+      <c r="D134" s="29">
+        <v>6044438</v>
       </c>
       <c r="E134" s="67" t="s">
         <v>238</v>
@@ -6992,8 +7030,8 @@
       <c r="C135" s="60" t="s">
         <v>216</v>
       </c>
-      <c r="D135" s="29" t="s">
-        <v>239</v>
+      <c r="D135" s="29">
+        <v>6222125</v>
       </c>
       <c r="E135" s="67" t="s">
         <v>240</v>
@@ -7015,8 +7053,8 @@
       <c r="C136" s="60" t="s">
         <v>171</v>
       </c>
-      <c r="D136" s="29" t="s">
-        <v>242</v>
+      <c r="D136" s="29">
+        <v>7463422</v>
       </c>
       <c r="E136" s="119" t="s">
         <v>243</v>
@@ -7038,8 +7076,8 @@
       <c r="C137" s="60" t="s">
         <v>171</v>
       </c>
-      <c r="D137" s="29" t="s">
-        <v>244</v>
+      <c r="D137" s="29">
+        <v>6800201</v>
       </c>
       <c r="E137" s="119" t="s">
         <v>245</v>
@@ -7061,8 +7099,8 @@
       <c r="C138" s="60" t="s">
         <v>171</v>
       </c>
-      <c r="D138" s="29" t="s">
-        <v>246</v>
+      <c r="D138" s="29">
+        <v>6043315</v>
       </c>
       <c r="E138" s="119" t="s">
         <v>247</v>
@@ -7084,8 +7122,8 @@
       <c r="C139" s="60" t="s">
         <v>171</v>
       </c>
-      <c r="D139" s="29" t="s">
-        <v>248</v>
+      <c r="D139" s="29">
+        <v>6260075</v>
       </c>
       <c r="E139" s="119" t="s">
         <v>249</v>
@@ -7107,8 +7145,8 @@
       <c r="C140" s="60" t="s">
         <v>171</v>
       </c>
-      <c r="D140" s="29" t="s">
-        <v>250</v>
+      <c r="D140" s="29">
+        <v>6260083</v>
       </c>
       <c r="E140" s="119" t="s">
         <v>251</v>
@@ -7130,8 +7168,8 @@
       <c r="C141" s="60" t="s">
         <v>171</v>
       </c>
-      <c r="D141" s="29" t="s">
-        <v>252</v>
+      <c r="D141" s="29">
+        <v>6099846</v>
       </c>
       <c r="E141" s="119" t="s">
         <v>253</v>
@@ -7145,7 +7183,7 @@
     </row>
     <row r="142" spans="1:7" ht="15.95" customHeight="1">
       <c r="A142" s="72" t="s">
-        <v>808</v>
+        <v>805</v>
       </c>
       <c r="B142" s="22" t="s">
         <v>28</v>
@@ -7168,7 +7206,7 @@
     </row>
     <row r="143" spans="1:7" ht="15.95" customHeight="1">
       <c r="A143" s="72" t="s">
-        <v>808</v>
+        <v>805</v>
       </c>
       <c r="B143" s="22" t="s">
         <v>28</v>
@@ -7191,7 +7229,7 @@
     </row>
     <row r="144" spans="1:7" ht="15.95" customHeight="1">
       <c r="A144" s="72" t="s">
-        <v>808</v>
+        <v>805</v>
       </c>
       <c r="B144" s="22" t="s">
         <v>28</v>
@@ -7214,7 +7252,7 @@
     </row>
     <row r="145" spans="1:7" ht="15.95" customHeight="1">
       <c r="A145" s="72" t="s">
-        <v>808</v>
+        <v>805</v>
       </c>
       <c r="B145" s="22" t="s">
         <v>28</v>
@@ -7237,7 +7275,7 @@
     </row>
     <row r="146" spans="1:7" ht="15.95" customHeight="1">
       <c r="A146" s="72" t="s">
-        <v>808</v>
+        <v>805</v>
       </c>
       <c r="B146" s="22" t="s">
         <v>28</v>
@@ -7260,7 +7298,7 @@
     </row>
     <row r="147" spans="1:7" ht="15.95" customHeight="1">
       <c r="A147" s="72" t="s">
-        <v>808</v>
+        <v>805</v>
       </c>
       <c r="B147" s="22" t="s">
         <v>153</v>
@@ -7283,7 +7321,7 @@
     </row>
     <row r="148" spans="1:7" ht="15.95" customHeight="1">
       <c r="A148" s="72" t="s">
-        <v>808</v>
+        <v>805</v>
       </c>
       <c r="B148" s="22" t="s">
         <v>161</v>
@@ -7306,7 +7344,7 @@
     </row>
     <row r="149" spans="1:7" ht="15.95" customHeight="1">
       <c r="A149" s="72" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="B149" s="22" t="s">
         <v>28</v>
@@ -7329,7 +7367,7 @@
     </row>
     <row r="150" spans="1:7" ht="15.95" customHeight="1">
       <c r="A150" s="72" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="B150" s="22" t="s">
         <v>28</v>
@@ -7352,7 +7390,7 @@
     </row>
     <row r="151" spans="1:7" ht="15.95" customHeight="1">
       <c r="A151" s="79" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="B151" s="38" t="s">
         <v>28</v>
@@ -7375,13 +7413,13 @@
     </row>
     <row r="152" spans="1:7" ht="15.95" customHeight="1">
       <c r="A152" s="72" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="B152" s="22" t="s">
         <v>8</v>
       </c>
       <c r="C152" s="60" t="s">
-        <v>266</v>
+        <v>828</v>
       </c>
       <c r="D152" s="44">
         <v>9908756</v>
@@ -7398,13 +7436,13 @@
     </row>
     <row r="153" spans="1:7" ht="15.95" customHeight="1">
       <c r="A153" s="72" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="B153" s="22" t="s">
         <v>8</v>
       </c>
       <c r="C153" s="60" t="s">
-        <v>266</v>
+        <v>828</v>
       </c>
       <c r="D153" s="44">
         <v>9908731</v>
@@ -7429,8 +7467,8 @@
       <c r="C154" s="76" t="s">
         <v>177</v>
       </c>
-      <c r="D154" s="29" t="s">
-        <v>280</v>
+      <c r="D154" s="29">
+        <v>6917187</v>
       </c>
       <c r="E154" s="67" t="s">
         <v>281</v>
@@ -7452,8 +7490,8 @@
       <c r="C155" s="76" t="s">
         <v>177</v>
       </c>
-      <c r="D155" s="29" t="s">
-        <v>282</v>
+      <c r="D155" s="29">
+        <v>6933226</v>
       </c>
       <c r="E155" s="67" t="s">
         <v>283</v>
@@ -7475,8 +7513,8 @@
       <c r="C156" s="60" t="s">
         <v>277</v>
       </c>
-      <c r="D156" s="29" t="s">
-        <v>278</v>
+      <c r="D156" s="29">
+        <v>6832865</v>
       </c>
       <c r="E156" s="67" t="s">
         <v>279</v>
@@ -7498,8 +7536,8 @@
       <c r="C157" s="60" t="s">
         <v>270</v>
       </c>
-      <c r="D157" s="29" t="s">
-        <v>271</v>
+      <c r="D157" s="29">
+        <v>6889147</v>
       </c>
       <c r="E157" s="67" t="s">
         <v>272</v>
@@ -7521,8 +7559,8 @@
       <c r="C158" s="60" t="s">
         <v>270</v>
       </c>
-      <c r="D158" s="29" t="s">
-        <v>273</v>
+      <c r="D158" s="29">
+        <v>6889154</v>
       </c>
       <c r="E158" s="67" t="s">
         <v>274</v>
@@ -7544,8 +7582,8 @@
       <c r="C159" s="60" t="s">
         <v>270</v>
       </c>
-      <c r="D159" s="29" t="s">
-        <v>275</v>
+      <c r="D159" s="29">
+        <v>6879817</v>
       </c>
       <c r="E159" s="67" t="s">
         <v>276</v>
@@ -7559,7 +7597,7 @@
     </row>
     <row r="160" spans="1:7" ht="15.95" customHeight="1">
       <c r="A160" s="72" t="s">
-        <v>818</v>
+        <v>822</v>
       </c>
       <c r="B160" s="22" t="s">
         <v>139</v>
@@ -7567,8 +7605,8 @@
       <c r="C160" s="76" t="s">
         <v>460</v>
       </c>
-      <c r="D160" s="28" t="s">
-        <v>461</v>
+      <c r="D160" s="28">
+        <v>5672688</v>
       </c>
       <c r="E160" s="66" t="s">
         <v>462</v>
@@ -7582,7 +7620,7 @@
     </row>
     <row r="161" spans="1:7" ht="15.95" customHeight="1">
       <c r="A161" s="72" t="s">
-        <v>818</v>
+        <v>822</v>
       </c>
       <c r="B161" s="22" t="s">
         <v>139</v>
@@ -7590,8 +7628,8 @@
       <c r="C161" s="76" t="s">
         <v>460</v>
       </c>
-      <c r="D161" s="28" t="s">
-        <v>463</v>
+      <c r="D161" s="28">
+        <v>9155333</v>
       </c>
       <c r="E161" s="66" t="s">
         <v>464</v>
@@ -7812,7 +7850,7 @@
     </row>
     <row r="171" spans="1:7">
       <c r="A171" s="72" t="s">
-        <v>811</v>
+        <v>808</v>
       </c>
       <c r="B171" s="89" t="s">
         <v>139</v>
@@ -7835,7 +7873,7 @@
     </row>
     <row r="172" spans="1:7" ht="15.95" customHeight="1">
       <c r="A172" s="72" t="s">
-        <v>812</v>
+        <v>809</v>
       </c>
       <c r="B172" s="89" t="s">
         <v>400</v>
@@ -7858,13 +7896,13 @@
     </row>
     <row r="173" spans="1:7" ht="15.95" customHeight="1">
       <c r="A173" s="72" t="s">
-        <v>812</v>
+        <v>809</v>
       </c>
       <c r="B173" s="89" t="s">
         <v>403</v>
       </c>
       <c r="C173" s="65" t="s">
-        <v>404</v>
+        <v>833</v>
       </c>
       <c r="D173" s="28">
         <v>6097147</v>
@@ -7881,7 +7919,7 @@
     </row>
     <row r="174" spans="1:7" ht="15.95" customHeight="1">
       <c r="A174" s="72" t="s">
-        <v>813</v>
+        <v>810</v>
       </c>
       <c r="B174" s="89" t="s">
         <v>400</v>
@@ -7904,13 +7942,13 @@
     </row>
     <row r="175" spans="1:7" ht="15.95" customHeight="1">
       <c r="A175" s="72" t="s">
-        <v>814</v>
+        <v>811</v>
       </c>
       <c r="B175" s="89" t="s">
         <v>403</v>
       </c>
       <c r="C175" s="65" t="s">
-        <v>404</v>
+        <v>833</v>
       </c>
       <c r="D175" s="28">
         <v>6097154</v>
@@ -7927,13 +7965,13 @@
     </row>
     <row r="176" spans="1:7" ht="15.95" customHeight="1">
       <c r="A176" s="72" t="s">
-        <v>814</v>
+        <v>811</v>
       </c>
       <c r="B176" s="89" t="s">
         <v>403</v>
       </c>
       <c r="C176" s="65" t="s">
-        <v>404</v>
+        <v>833</v>
       </c>
       <c r="D176" s="28">
         <v>6097162</v>
@@ -7958,8 +7996,8 @@
       <c r="C177" s="65" t="s">
         <v>298</v>
       </c>
-      <c r="D177" s="28" t="s">
-        <v>299</v>
+      <c r="D177" s="28">
+        <v>8624403</v>
       </c>
       <c r="E177" s="66" t="s">
         <v>300</v>
@@ -7981,8 +8019,8 @@
       <c r="C178" s="65" t="s">
         <v>298</v>
       </c>
-      <c r="D178" s="28" t="s">
-        <v>301</v>
+      <c r="D178" s="28">
+        <v>5273347</v>
       </c>
       <c r="E178" s="66" t="s">
         <v>302</v>
@@ -8004,8 +8042,8 @@
       <c r="C179" s="65" t="s">
         <v>298</v>
       </c>
-      <c r="D179" s="28" t="s">
-        <v>303</v>
+      <c r="D179" s="28">
+        <v>8624411</v>
       </c>
       <c r="E179" s="66" t="s">
         <v>304</v>
@@ -8027,8 +8065,8 @@
       <c r="C180" s="65" t="s">
         <v>82</v>
       </c>
-      <c r="D180" s="29" t="s">
-        <v>306</v>
+      <c r="D180" s="29">
+        <v>6259358</v>
       </c>
       <c r="E180" s="119" t="s">
         <v>307</v>
@@ -8050,8 +8088,8 @@
       <c r="C181" s="65" t="s">
         <v>82</v>
       </c>
-      <c r="D181" s="29" t="s">
-        <v>308</v>
+      <c r="D181" s="29">
+        <v>6259366</v>
       </c>
       <c r="E181" s="119" t="s">
         <v>309</v>
@@ -8073,8 +8111,8 @@
       <c r="C182" s="65" t="s">
         <v>311</v>
       </c>
-      <c r="D182" s="29" t="s">
-        <v>312</v>
+      <c r="D182" s="29">
+        <v>6118968</v>
       </c>
       <c r="E182" s="67" t="s">
         <v>313</v>
@@ -8096,8 +8134,8 @@
       <c r="C183" s="65" t="s">
         <v>311</v>
       </c>
-      <c r="D183" s="29" t="s">
-        <v>314</v>
+      <c r="D183" s="29">
+        <v>6011940</v>
       </c>
       <c r="E183" s="67" t="s">
         <v>315</v>
@@ -8119,8 +8157,8 @@
       <c r="C184" s="65" t="s">
         <v>311</v>
       </c>
-      <c r="D184" s="29" t="s">
-        <v>316</v>
+      <c r="D184" s="29">
+        <v>6213058</v>
       </c>
       <c r="E184" s="67" t="s">
         <v>317</v>
@@ -8142,8 +8180,8 @@
       <c r="C185" s="65" t="s">
         <v>311</v>
       </c>
-      <c r="D185" s="29" t="s">
-        <v>318</v>
+      <c r="D185" s="29">
+        <v>6150631</v>
       </c>
       <c r="E185" s="67" t="s">
         <v>319</v>
@@ -8165,8 +8203,8 @@
       <c r="C186" s="65" t="s">
         <v>311</v>
       </c>
-      <c r="D186" s="29" t="s">
-        <v>320</v>
+      <c r="D186" s="29">
+        <v>6780890</v>
       </c>
       <c r="E186" s="67" t="s">
         <v>321</v>
@@ -8188,8 +8226,8 @@
       <c r="C187" s="65" t="s">
         <v>311</v>
       </c>
-      <c r="D187" s="29" t="s">
-        <v>322</v>
+      <c r="D187" s="29">
+        <v>6780973</v>
       </c>
       <c r="E187" s="67" t="s">
         <v>323</v>
@@ -8211,8 +8249,8 @@
       <c r="C188" s="65" t="s">
         <v>311</v>
       </c>
-      <c r="D188" s="29" t="s">
-        <v>324</v>
+      <c r="D188" s="29">
+        <v>6768598</v>
       </c>
       <c r="E188" s="67" t="s">
         <v>325</v>
@@ -8234,8 +8272,8 @@
       <c r="C189" s="60" t="s">
         <v>311</v>
       </c>
-      <c r="D189" s="29" t="s">
-        <v>326</v>
+      <c r="D189" s="29">
+        <v>6960179</v>
       </c>
       <c r="E189" s="67" t="s">
         <v>327</v>
@@ -8257,8 +8295,8 @@
       <c r="C190" s="60" t="s">
         <v>311</v>
       </c>
-      <c r="D190" s="29" t="s">
-        <v>328</v>
+      <c r="D190" s="29">
+        <v>6119743</v>
       </c>
       <c r="E190" s="67" t="s">
         <v>329</v>
@@ -8280,8 +8318,8 @@
       <c r="C191" s="60" t="s">
         <v>311</v>
       </c>
-      <c r="D191" s="29" t="s">
-        <v>330</v>
+      <c r="D191" s="29">
+        <v>7757492</v>
       </c>
       <c r="E191" s="67" t="s">
         <v>331</v>
@@ -8303,8 +8341,8 @@
       <c r="C192" s="98" t="s">
         <v>311</v>
       </c>
-      <c r="D192" s="106" t="s">
-        <v>332</v>
+      <c r="D192" s="106">
+        <v>7755454</v>
       </c>
       <c r="E192" s="100" t="s">
         <v>333</v>
@@ -8326,8 +8364,8 @@
       <c r="C193" s="98" t="s">
         <v>311</v>
       </c>
-      <c r="D193" s="106" t="s">
-        <v>334</v>
+      <c r="D193" s="106">
+        <v>7755462</v>
       </c>
       <c r="E193" s="100" t="s">
         <v>335</v>
@@ -8349,8 +8387,8 @@
       <c r="C194" s="60" t="s">
         <v>311</v>
       </c>
-      <c r="D194" s="29" t="s">
-        <v>336</v>
+      <c r="D194" s="29">
+        <v>6005868</v>
       </c>
       <c r="E194" s="67" t="s">
         <v>337</v>
@@ -8372,8 +8410,8 @@
       <c r="C195" s="60" t="s">
         <v>311</v>
       </c>
-      <c r="D195" s="29" t="s">
-        <v>338</v>
+      <c r="D195" s="29">
+        <v>6242479</v>
       </c>
       <c r="E195" s="67" t="s">
         <v>339</v>
@@ -8395,8 +8433,8 @@
       <c r="C196" s="101" t="s">
         <v>311</v>
       </c>
-      <c r="D196" s="104" t="s">
-        <v>340</v>
+      <c r="D196" s="104">
+        <v>6330191</v>
       </c>
       <c r="E196" s="105" t="s">
         <v>341</v>
@@ -8418,8 +8456,8 @@
       <c r="C197" s="146" t="s">
         <v>311</v>
       </c>
-      <c r="D197" s="104" t="s">
-        <v>342</v>
+      <c r="D197" s="104">
+        <v>6330183</v>
       </c>
       <c r="E197" s="105" t="s">
         <v>343</v>
@@ -8441,8 +8479,8 @@
       <c r="C198" s="62" t="s">
         <v>311</v>
       </c>
-      <c r="D198" s="29" t="s">
-        <v>344</v>
+      <c r="D198" s="29">
+        <v>6287706</v>
       </c>
       <c r="E198" s="67" t="s">
         <v>345</v>
@@ -8464,8 +8502,8 @@
       <c r="C199" s="63" t="s">
         <v>311</v>
       </c>
-      <c r="D199" s="78" t="s">
-        <v>346</v>
+      <c r="D199" s="78">
+        <v>6287714</v>
       </c>
       <c r="E199" s="90" t="s">
         <v>347</v>
@@ -8487,8 +8525,8 @@
       <c r="C200" s="63" t="s">
         <v>311</v>
       </c>
-      <c r="D200" s="29" t="s">
-        <v>348</v>
+      <c r="D200" s="29">
+        <v>6099234</v>
       </c>
       <c r="E200" s="67" t="s">
         <v>349</v>
@@ -9054,7 +9092,7 @@
     </row>
     <row r="225" spans="1:7" ht="15">
       <c r="A225" s="72" t="s">
-        <v>824</v>
+        <v>819</v>
       </c>
       <c r="B225" s="22" t="s">
         <v>748</v>
@@ -9062,8 +9100,8 @@
       <c r="C225" s="60" t="s">
         <v>445</v>
       </c>
-      <c r="D225" s="29" t="s">
-        <v>446</v>
+      <c r="D225" s="29">
+        <v>9817700</v>
       </c>
       <c r="E225" s="67" t="s">
         <v>445</v>
@@ -9077,7 +9115,7 @@
     </row>
     <row r="226" spans="1:7" ht="15">
       <c r="A226" s="72" t="s">
-        <v>824</v>
+        <v>819</v>
       </c>
       <c r="B226" s="22" t="s">
         <v>28</v>
@@ -9085,8 +9123,8 @@
       <c r="C226" s="60" t="s">
         <v>440</v>
       </c>
-      <c r="D226" s="29" t="s">
-        <v>441</v>
+      <c r="D226" s="29">
+        <v>9998914</v>
       </c>
       <c r="E226" s="67" t="s">
         <v>440</v>
@@ -9100,7 +9138,7 @@
     </row>
     <row r="227" spans="1:7" ht="15">
       <c r="A227" s="72" t="s">
-        <v>824</v>
+        <v>819</v>
       </c>
       <c r="B227" s="22" t="s">
         <v>13</v>
@@ -9108,8 +9146,8 @@
       <c r="C227" s="60" t="s">
         <v>442</v>
       </c>
-      <c r="D227" s="29" t="s">
-        <v>443</v>
+      <c r="D227" s="29">
+        <v>7382887</v>
       </c>
       <c r="E227" s="67" t="s">
         <v>444</v>
@@ -9123,7 +9161,7 @@
     </row>
     <row r="228" spans="1:7" ht="15">
       <c r="A228" s="72" t="s">
-        <v>825</v>
+        <v>820</v>
       </c>
       <c r="B228" s="22" t="s">
         <v>450</v>
@@ -9131,8 +9169,8 @@
       <c r="C228" s="60" t="s">
         <v>451</v>
       </c>
-      <c r="D228" s="29" t="s">
-        <v>452</v>
+      <c r="D228" s="29">
+        <v>9310128</v>
       </c>
       <c r="E228" s="66" t="s">
         <v>453</v>
@@ -9146,7 +9184,7 @@
     </row>
     <row r="229" spans="1:7" ht="15">
       <c r="A229" s="72" t="s">
-        <v>825</v>
+        <v>820</v>
       </c>
       <c r="B229" s="22" t="s">
         <v>450</v>
@@ -9154,8 +9192,8 @@
       <c r="C229" s="60" t="s">
         <v>451</v>
       </c>
-      <c r="D229" s="29" t="s">
-        <v>454</v>
+      <c r="D229" s="29">
+        <v>9310136</v>
       </c>
       <c r="E229" s="66" t="s">
         <v>455</v>
@@ -9169,7 +9207,7 @@
     </row>
     <row r="230" spans="1:7" ht="15">
       <c r="A230" s="72" t="s">
-        <v>825</v>
+        <v>820</v>
       </c>
       <c r="B230" s="22" t="s">
         <v>450</v>
@@ -9177,8 +9215,8 @@
       <c r="C230" s="60" t="s">
         <v>451</v>
       </c>
-      <c r="D230" s="29" t="s">
-        <v>456</v>
+      <c r="D230" s="29">
+        <v>5583117</v>
       </c>
       <c r="E230" s="66" t="s">
         <v>457</v>
@@ -9192,7 +9230,7 @@
     </row>
     <row r="231" spans="1:7" ht="15">
       <c r="A231" s="72" t="s">
-        <v>825</v>
+        <v>820</v>
       </c>
       <c r="B231" s="22" t="s">
         <v>450</v>
@@ -9200,8 +9238,8 @@
       <c r="C231" s="60" t="s">
         <v>451</v>
       </c>
-      <c r="D231" s="29" t="s">
-        <v>458</v>
+      <c r="D231" s="29">
+        <v>5553961</v>
       </c>
       <c r="E231" s="66" t="s">
         <v>459</v>
@@ -9215,7 +9253,7 @@
     </row>
     <row r="232" spans="1:7" ht="15">
       <c r="A232" s="72" t="s">
-        <v>825</v>
+        <v>820</v>
       </c>
       <c r="B232" s="38" t="s">
         <v>450</v>
@@ -9223,8 +9261,8 @@
       <c r="C232" s="60" t="s">
         <v>451</v>
       </c>
-      <c r="D232" s="29" t="s">
-        <v>456</v>
+      <c r="D232" s="29">
+        <v>5583117</v>
       </c>
       <c r="E232" s="66" t="s">
         <v>457</v>
@@ -9238,7 +9276,7 @@
     </row>
     <row r="233" spans="1:7" ht="15">
       <c r="A233" s="72" t="s">
-        <v>825</v>
+        <v>820</v>
       </c>
       <c r="B233" s="43" t="s">
         <v>139</v>
@@ -9246,8 +9284,8 @@
       <c r="C233" s="61" t="s">
         <v>447</v>
       </c>
-      <c r="D233" s="29" t="s">
-        <v>448</v>
+      <c r="D233" s="29">
+        <v>5338751</v>
       </c>
       <c r="E233" s="66" t="s">
         <v>449</v>
@@ -9269,8 +9307,8 @@
       <c r="C234" s="61" t="s">
         <v>490</v>
       </c>
-      <c r="D234" s="29" t="s">
-        <v>493</v>
+      <c r="D234" s="29">
+        <v>6825521</v>
       </c>
       <c r="E234" s="67" t="s">
         <v>494</v>
@@ -9292,8 +9330,8 @@
       <c r="C235" s="60" t="s">
         <v>490</v>
       </c>
-      <c r="D235" s="29" t="s">
-        <v>495</v>
+      <c r="D235" s="29">
+        <v>6560839</v>
       </c>
       <c r="E235" s="67" t="s">
         <v>496</v>
@@ -9315,8 +9353,8 @@
       <c r="C236" s="60" t="s">
         <v>490</v>
       </c>
-      <c r="D236" s="29" t="s">
-        <v>497</v>
+      <c r="D236" s="29">
+        <v>6944751</v>
       </c>
       <c r="E236" s="67" t="s">
         <v>498</v>
@@ -9338,8 +9376,8 @@
       <c r="C237" s="60" t="s">
         <v>490</v>
       </c>
-      <c r="D237" s="29" t="s">
-        <v>499</v>
+      <c r="D237" s="29">
+        <v>6915140</v>
       </c>
       <c r="E237" s="67" t="s">
         <v>500</v>
@@ -9361,8 +9399,8 @@
       <c r="C238" s="60" t="s">
         <v>490</v>
       </c>
-      <c r="D238" s="29" t="s">
-        <v>503</v>
+      <c r="D238" s="29">
+        <v>6915363</v>
       </c>
       <c r="E238" s="67" t="s">
         <v>504</v>
@@ -9384,8 +9422,8 @@
       <c r="C239" s="61" t="s">
         <v>466</v>
       </c>
-      <c r="D239" s="29" t="s">
-        <v>471</v>
+      <c r="D239" s="29">
+        <v>6039867</v>
       </c>
       <c r="E239" s="67" t="s">
         <v>472</v>
@@ -9407,8 +9445,8 @@
       <c r="C240" s="60" t="s">
         <v>466</v>
       </c>
-      <c r="D240" s="29" t="s">
-        <v>473</v>
+      <c r="D240" s="29">
+        <v>6524454</v>
       </c>
       <c r="E240" s="67" t="s">
         <v>474</v>
@@ -9430,8 +9468,8 @@
       <c r="C241" s="60" t="s">
         <v>466</v>
       </c>
-      <c r="D241" s="29" t="s">
-        <v>475</v>
+      <c r="D241" s="29">
+        <v>6932194</v>
       </c>
       <c r="E241" s="67" t="s">
         <v>476</v>
@@ -9453,8 +9491,8 @@
       <c r="C242" s="60" t="s">
         <v>466</v>
       </c>
-      <c r="D242" s="29" t="s">
-        <v>477</v>
+      <c r="D242" s="29">
+        <v>6932202</v>
       </c>
       <c r="E242" s="67" t="s">
         <v>478</v>
@@ -9476,8 +9514,8 @@
       <c r="C243" s="60" t="s">
         <v>466</v>
       </c>
-      <c r="D243" s="29" t="s">
-        <v>479</v>
+      <c r="D243" s="29">
+        <v>6932228</v>
       </c>
       <c r="E243" s="67" t="s">
         <v>480</v>
@@ -9499,8 +9537,8 @@
       <c r="C244" s="60" t="s">
         <v>466</v>
       </c>
-      <c r="D244" s="29" t="s">
-        <v>481</v>
+      <c r="D244" s="29">
+        <v>6932210</v>
       </c>
       <c r="E244" s="67" t="s">
         <v>482</v>
@@ -9522,8 +9560,8 @@
       <c r="C245" s="65" t="s">
         <v>466</v>
       </c>
-      <c r="D245" s="29" t="s">
-        <v>483</v>
+      <c r="D245" s="29">
+        <v>6809269</v>
       </c>
       <c r="E245" s="67" t="s">
         <v>484</v>
@@ -9545,8 +9583,8 @@
       <c r="C246" s="65" t="s">
         <v>466</v>
       </c>
-      <c r="D246" s="29" t="s">
-        <v>485</v>
+      <c r="D246" s="29">
+        <v>6562017</v>
       </c>
       <c r="E246" s="67" t="s">
         <v>486</v>
@@ -9729,8 +9767,8 @@
       <c r="C254" s="60" t="s">
         <v>542</v>
       </c>
-      <c r="D254" s="29" t="s">
-        <v>543</v>
+      <c r="D254" s="29">
+        <v>7355586</v>
       </c>
       <c r="E254" s="67" t="s">
         <v>544</v>
@@ -9752,8 +9790,8 @@
       <c r="C255" s="60" t="s">
         <v>542</v>
       </c>
-      <c r="D255" s="29" t="s">
-        <v>545</v>
+      <c r="D255" s="29">
+        <v>7394023</v>
       </c>
       <c r="E255" s="67" t="s">
         <v>546</v>
@@ -9775,8 +9813,8 @@
       <c r="C256" s="60" t="s">
         <v>542</v>
       </c>
-      <c r="D256" s="29" t="s">
-        <v>547</v>
+      <c r="D256" s="29">
+        <v>7394080</v>
       </c>
       <c r="E256" s="67" t="s">
         <v>548</v>
@@ -9798,8 +9836,8 @@
       <c r="C257" s="60" t="s">
         <v>542</v>
       </c>
-      <c r="D257" s="29" t="s">
-        <v>549</v>
+      <c r="D257" s="29">
+        <v>7394049</v>
       </c>
       <c r="E257" s="67" t="s">
         <v>550</v>
@@ -9821,8 +9859,8 @@
       <c r="C258" s="60" t="s">
         <v>542</v>
       </c>
-      <c r="D258" s="29" t="s">
-        <v>551</v>
+      <c r="D258" s="29">
+        <v>7394064</v>
       </c>
       <c r="E258" s="67" t="s">
         <v>552</v>
@@ -9844,8 +9882,8 @@
       <c r="C259" s="60" t="s">
         <v>542</v>
       </c>
-      <c r="D259" s="29" t="s">
-        <v>553</v>
+      <c r="D259" s="29">
+        <v>7394072</v>
       </c>
       <c r="E259" s="67" t="s">
         <v>554</v>
@@ -9867,8 +9905,8 @@
       <c r="C260" s="60" t="s">
         <v>542</v>
       </c>
-      <c r="D260" s="29" t="s">
-        <v>555</v>
+      <c r="D260" s="29">
+        <v>7394056</v>
       </c>
       <c r="E260" s="67" t="s">
         <v>556</v>
@@ -9890,8 +9928,8 @@
       <c r="C261" s="60" t="s">
         <v>542</v>
       </c>
-      <c r="D261" s="29" t="s">
-        <v>557</v>
+      <c r="D261" s="29">
+        <v>7394031</v>
       </c>
       <c r="E261" s="67" t="s">
         <v>558</v>
@@ -9913,8 +9951,8 @@
       <c r="C262" s="60" t="s">
         <v>542</v>
       </c>
-      <c r="D262" s="29" t="s">
-        <v>559</v>
+      <c r="D262" s="29">
+        <v>6088294</v>
       </c>
       <c r="E262" s="67" t="s">
         <v>560</v>
@@ -9936,8 +9974,8 @@
       <c r="C263" s="60" t="s">
         <v>515</v>
       </c>
-      <c r="D263" s="29" t="s">
-        <v>516</v>
+      <c r="D263" s="29">
+        <v>7383919</v>
       </c>
       <c r="E263" s="67" t="s">
         <v>517</v>
@@ -9959,8 +9997,8 @@
       <c r="C264" s="64" t="s">
         <v>515</v>
       </c>
-      <c r="D264" s="48" t="s">
-        <v>518</v>
+      <c r="D264" s="48">
+        <v>7388728</v>
       </c>
       <c r="E264" s="67" t="s">
         <v>519</v>
@@ -9982,8 +10020,8 @@
       <c r="C265" s="61" t="s">
         <v>515</v>
       </c>
-      <c r="D265" s="29" t="s">
-        <v>520</v>
+      <c r="D265" s="29">
+        <v>7394254</v>
       </c>
       <c r="E265" s="67" t="s">
         <v>521</v>
@@ -10005,8 +10043,8 @@
       <c r="C266" s="60" t="s">
         <v>515</v>
       </c>
-      <c r="D266" s="78" t="s">
-        <v>522</v>
+      <c r="D266" s="78">
+        <v>7351775</v>
       </c>
       <c r="E266" s="67" t="s">
         <v>523</v>
@@ -10028,8 +10066,8 @@
       <c r="C267" s="60" t="s">
         <v>515</v>
       </c>
-      <c r="D267" s="29" t="s">
-        <v>524</v>
+      <c r="D267" s="29">
+        <v>7351809</v>
       </c>
       <c r="E267" s="67" t="s">
         <v>525</v>
@@ -10051,8 +10089,8 @@
       <c r="C268" s="61" t="s">
         <v>515</v>
       </c>
-      <c r="D268" s="29" t="s">
-        <v>526</v>
+      <c r="D268" s="29">
+        <v>7351791</v>
       </c>
       <c r="E268" s="67" t="s">
         <v>527</v>
@@ -10074,8 +10112,8 @@
       <c r="C269" s="61" t="s">
         <v>515</v>
       </c>
-      <c r="D269" s="29" t="s">
-        <v>528</v>
+      <c r="D269" s="29">
+        <v>7388736</v>
       </c>
       <c r="E269" s="67" t="s">
         <v>529</v>
@@ -10097,8 +10135,8 @@
       <c r="C270" s="61" t="s">
         <v>515</v>
       </c>
-      <c r="D270" s="29" t="s">
-        <v>530</v>
+      <c r="D270" s="29">
+        <v>7383901</v>
       </c>
       <c r="E270" s="67" t="s">
         <v>531</v>
@@ -10120,8 +10158,8 @@
       <c r="C271" s="61" t="s">
         <v>515</v>
       </c>
-      <c r="D271" s="29" t="s">
-        <v>532</v>
+      <c r="D271" s="29">
+        <v>7351734</v>
       </c>
       <c r="E271" s="67" t="s">
         <v>533</v>
@@ -10143,8 +10181,8 @@
       <c r="C272" s="61" t="s">
         <v>515</v>
       </c>
-      <c r="D272" s="29" t="s">
-        <v>534</v>
+      <c r="D272" s="29">
+        <v>7394270</v>
       </c>
       <c r="E272" s="67" t="s">
         <v>535</v>
@@ -10166,8 +10204,8 @@
       <c r="C273" s="60" t="s">
         <v>515</v>
       </c>
-      <c r="D273" s="48" t="s">
-        <v>536</v>
+      <c r="D273" s="48">
+        <v>7394262</v>
       </c>
       <c r="E273" s="113" t="s">
         <v>537</v>
@@ -10189,8 +10227,8 @@
       <c r="C274" s="60" t="s">
         <v>515</v>
       </c>
-      <c r="D274" s="48" t="s">
-        <v>538</v>
+      <c r="D274" s="48">
+        <v>7394247</v>
       </c>
       <c r="E274" s="113" t="s">
         <v>539</v>
@@ -10212,8 +10250,8 @@
       <c r="C275" s="60" t="s">
         <v>515</v>
       </c>
-      <c r="D275" s="48" t="s">
-        <v>540</v>
+      <c r="D275" s="48">
+        <v>6059691</v>
       </c>
       <c r="E275" s="113" t="s">
         <v>541</v>
@@ -10411,13 +10449,13 @@
     </row>
     <row r="284" spans="1:7">
       <c r="A284" s="80" t="s">
-        <v>815</v>
+        <v>821</v>
       </c>
       <c r="B284" s="22" t="s">
         <v>28</v>
       </c>
       <c r="C284" s="65" t="s">
-        <v>368</v>
+        <v>829</v>
       </c>
       <c r="D284" s="28">
         <v>6284885</v>
@@ -10434,13 +10472,13 @@
     </row>
     <row r="285" spans="1:7">
       <c r="A285" s="80" t="s">
-        <v>815</v>
+        <v>821</v>
       </c>
       <c r="B285" s="22" t="s">
         <v>28</v>
       </c>
       <c r="C285" s="65" t="s">
-        <v>368</v>
+        <v>829</v>
       </c>
       <c r="D285" s="28">
         <v>6334722</v>
@@ -10457,13 +10495,13 @@
     </row>
     <row r="286" spans="1:7">
       <c r="A286" s="80" t="s">
-        <v>815</v>
+        <v>821</v>
       </c>
       <c r="B286" s="22" t="s">
         <v>371</v>
       </c>
       <c r="C286" s="65" t="s">
-        <v>372</v>
+        <v>830</v>
       </c>
       <c r="D286" s="28">
         <v>6180554</v>
@@ -10480,13 +10518,13 @@
     </row>
     <row r="287" spans="1:7">
       <c r="A287" s="80" t="s">
-        <v>815</v>
+        <v>821</v>
       </c>
       <c r="B287" s="22" t="s">
         <v>371</v>
       </c>
       <c r="C287" s="65" t="s">
-        <v>372</v>
+        <v>830</v>
       </c>
       <c r="D287" s="28">
         <v>6294736</v>
@@ -10503,13 +10541,13 @@
     </row>
     <row r="288" spans="1:7">
       <c r="A288" s="80" t="s">
-        <v>815</v>
+        <v>821</v>
       </c>
       <c r="B288" s="22" t="s">
         <v>371</v>
       </c>
       <c r="C288" s="65" t="s">
-        <v>372</v>
+        <v>830</v>
       </c>
       <c r="D288" s="28">
         <v>6294744</v>
@@ -10526,13 +10564,13 @@
     </row>
     <row r="289" spans="1:7">
       <c r="A289" s="80" t="s">
-        <v>815</v>
+        <v>821</v>
       </c>
       <c r="B289" s="22" t="s">
         <v>371</v>
       </c>
       <c r="C289" s="65" t="s">
-        <v>372</v>
+        <v>830</v>
       </c>
       <c r="D289" s="28">
         <v>6180562</v>
@@ -10549,13 +10587,13 @@
     </row>
     <row r="290" spans="1:7">
       <c r="A290" s="80" t="s">
-        <v>815</v>
+        <v>821</v>
       </c>
       <c r="B290" s="22" t="s">
         <v>371</v>
       </c>
       <c r="C290" s="65" t="s">
-        <v>372</v>
+        <v>830</v>
       </c>
       <c r="D290" s="28">
         <v>6317792</v>
@@ -10572,13 +10610,13 @@
     </row>
     <row r="291" spans="1:7">
       <c r="A291" s="72" t="s">
-        <v>820</v>
+        <v>815</v>
       </c>
       <c r="B291" s="22" t="s">
         <v>73</v>
       </c>
       <c r="C291" s="65" t="s">
-        <v>574</v>
+        <v>835</v>
       </c>
       <c r="D291" s="28">
         <v>6349068</v>
@@ -10595,7 +10633,7 @@
     </row>
     <row r="292" spans="1:7">
       <c r="A292" s="72" t="s">
-        <v>822</v>
+        <v>817</v>
       </c>
       <c r="B292" s="22" t="s">
         <v>139</v>
@@ -10618,7 +10656,7 @@
     </row>
     <row r="293" spans="1:7">
       <c r="A293" s="72" t="s">
-        <v>821</v>
+        <v>816</v>
       </c>
       <c r="B293" s="22" t="s">
         <v>139</v>
@@ -10626,8 +10664,8 @@
       <c r="C293" s="65" t="s">
         <v>576</v>
       </c>
-      <c r="D293" s="29" t="s">
-        <v>577</v>
+      <c r="D293" s="29">
+        <v>7355842</v>
       </c>
       <c r="E293" s="67" t="s">
         <v>578</v>
@@ -10641,7 +10679,7 @@
     </row>
     <row r="294" spans="1:7">
       <c r="A294" s="72" t="s">
-        <v>819</v>
+        <v>814</v>
       </c>
       <c r="B294" s="22" t="s">
         <v>579</v>
@@ -10649,8 +10687,8 @@
       <c r="C294" s="65" t="s">
         <v>580</v>
       </c>
-      <c r="D294" s="29" t="s">
-        <v>581</v>
+      <c r="D294" s="29">
+        <v>7357608</v>
       </c>
       <c r="E294" s="67" t="s">
         <v>582</v>
@@ -10664,7 +10702,7 @@
     </row>
     <row r="295" spans="1:7">
       <c r="A295" s="72" t="s">
-        <v>819</v>
+        <v>814</v>
       </c>
       <c r="B295" s="22" t="s">
         <v>579</v>
@@ -10672,8 +10710,8 @@
       <c r="C295" s="64" t="s">
         <v>580</v>
       </c>
-      <c r="D295" s="29" t="s">
-        <v>583</v>
+      <c r="D295" s="29">
+        <v>7373803</v>
       </c>
       <c r="E295" s="67" t="s">
         <v>584</v>
@@ -10695,8 +10733,8 @@
       <c r="C296" s="64" t="s">
         <v>588</v>
       </c>
-      <c r="D296" s="29" t="s">
-        <v>589</v>
+      <c r="D296" s="29">
+        <v>6262964</v>
       </c>
       <c r="E296" s="67" t="s">
         <v>590</v>
@@ -10718,8 +10756,8 @@
       <c r="C297" s="124" t="s">
         <v>588</v>
       </c>
-      <c r="D297" s="96" t="s">
-        <v>591</v>
+      <c r="D297" s="96">
+        <v>5703707</v>
       </c>
       <c r="E297" s="97" t="s">
         <v>592</v>
@@ -10733,19 +10771,19 @@
     </row>
     <row r="298" spans="1:7">
       <c r="A298" s="72" t="s">
-        <v>790</v>
+        <v>787</v>
       </c>
       <c r="B298" s="145" t="s">
         <v>732</v>
       </c>
       <c r="C298" s="124" t="s">
-        <v>787</v>
-      </c>
-      <c r="D298" s="96" t="s">
-        <v>788</v>
+        <v>785</v>
+      </c>
+      <c r="D298" s="96">
+        <v>7473355</v>
       </c>
       <c r="E298" s="97" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
       <c r="F298" s="85">
         <v>0.32</v>
@@ -10787,8 +10825,8 @@
       <c r="C300" s="64" t="s">
         <v>594</v>
       </c>
-      <c r="D300" s="28" t="s">
-        <v>595</v>
+      <c r="D300" s="28">
+        <v>5431705</v>
       </c>
       <c r="E300" s="66" t="s">
         <v>596</v>
@@ -10810,8 +10848,8 @@
       <c r="C301" s="64" t="s">
         <v>594</v>
       </c>
-      <c r="D301" s="28" t="s">
-        <v>597</v>
+      <c r="D301" s="28">
+        <v>5431713</v>
       </c>
       <c r="E301" s="66" t="s">
         <v>598</v>
@@ -10831,10 +10869,10 @@
         <v>18</v>
       </c>
       <c r="C302" s="147" t="s">
-        <v>610</v>
-      </c>
-      <c r="D302" s="29" t="s">
-        <v>611</v>
+        <v>667</v>
+      </c>
+      <c r="D302" s="29">
+        <v>7390716</v>
       </c>
       <c r="E302" s="67" t="s">
         <v>612</v>
@@ -10854,10 +10892,10 @@
         <v>18</v>
       </c>
       <c r="C303" s="147" t="s">
-        <v>610</v>
-      </c>
-      <c r="D303" s="29" t="s">
-        <v>613</v>
+        <v>667</v>
+      </c>
+      <c r="D303" s="29">
+        <v>6255968</v>
       </c>
       <c r="E303" s="67" t="s">
         <v>614</v>
@@ -10876,14 +10914,14 @@
       <c r="B304" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="C304" s="121" t="s">
-        <v>610</v>
-      </c>
-      <c r="D304" s="29" t="s">
+      <c r="C304" s="147" t="s">
+        <v>667</v>
+      </c>
+      <c r="D304" s="29">
+        <v>6323048</v>
+      </c>
+      <c r="E304" s="67" t="s">
         <v>769</v>
-      </c>
-      <c r="E304" s="67" t="s">
-        <v>770</v>
       </c>
       <c r="F304" s="73">
         <v>0.159</v>
@@ -10899,11 +10937,11 @@
       <c r="B305" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="C305" s="121" t="s">
-        <v>610</v>
-      </c>
-      <c r="D305" s="29" t="s">
-        <v>617</v>
+      <c r="C305" s="147" t="s">
+        <v>667</v>
+      </c>
+      <c r="D305" s="29">
+        <v>6029041</v>
       </c>
       <c r="E305" s="67" t="s">
         <v>618</v>
@@ -10922,14 +10960,14 @@
       <c r="B306" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="C306" s="121" t="s">
-        <v>610</v>
-      </c>
-      <c r="D306" s="29" t="s">
-        <v>771</v>
+      <c r="C306" s="147" t="s">
+        <v>667</v>
+      </c>
+      <c r="D306" s="29">
+        <v>6384727</v>
       </c>
       <c r="E306" s="67" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="F306" s="73">
         <v>0.159</v>
@@ -10945,11 +10983,11 @@
       <c r="B307" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="C307" s="61" t="s">
-        <v>599</v>
-      </c>
-      <c r="D307" s="28" t="s">
-        <v>600</v>
+      <c r="C307" s="147" t="s">
+        <v>667</v>
+      </c>
+      <c r="D307" s="28">
+        <v>3886884</v>
       </c>
       <c r="E307" s="66" t="s">
         <v>601</v>
@@ -10968,11 +11006,11 @@
       <c r="B308" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="C308" s="61" t="s">
-        <v>599</v>
-      </c>
-      <c r="D308" s="28" t="s">
-        <v>602</v>
+      <c r="C308" s="147" t="s">
+        <v>667</v>
+      </c>
+      <c r="D308" s="28">
+        <v>5346820</v>
       </c>
       <c r="E308" s="66" t="s">
         <v>603</v>
@@ -10991,11 +11029,11 @@
       <c r="B309" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="C309" s="61" t="s">
-        <v>599</v>
-      </c>
-      <c r="D309" s="74" t="s">
-        <v>604</v>
+      <c r="C309" s="147" t="s">
+        <v>667</v>
+      </c>
+      <c r="D309" s="74">
+        <v>5346846</v>
       </c>
       <c r="E309" s="75" t="s">
         <v>605</v>
@@ -11014,11 +11052,11 @@
       <c r="B310" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="C310" s="61" t="s">
-        <v>599</v>
-      </c>
-      <c r="D310" s="28" t="s">
-        <v>606</v>
+      <c r="C310" s="147" t="s">
+        <v>667</v>
+      </c>
+      <c r="D310" s="28">
+        <v>8883629</v>
       </c>
       <c r="E310" s="66" t="s">
         <v>607</v>
@@ -11037,11 +11075,11 @@
       <c r="B311" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="C311" s="61" t="s">
-        <v>599</v>
-      </c>
-      <c r="D311" s="28" t="s">
-        <v>608</v>
+      <c r="C311" s="147" t="s">
+        <v>667</v>
+      </c>
+      <c r="D311" s="28">
+        <v>8883637</v>
       </c>
       <c r="E311" s="66" t="s">
         <v>609</v>
@@ -11060,11 +11098,11 @@
       <c r="B312" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="C312" s="61" t="s">
-        <v>599</v>
-      </c>
-      <c r="D312" s="28" t="s">
-        <v>619</v>
+      <c r="C312" s="147" t="s">
+        <v>667</v>
+      </c>
+      <c r="D312" s="28">
+        <v>5593025</v>
       </c>
       <c r="E312" s="66" t="s">
         <v>620</v>
@@ -11086,8 +11124,8 @@
       <c r="C313" s="95" t="s">
         <v>634</v>
       </c>
-      <c r="D313" s="29" t="s">
-        <v>635</v>
+      <c r="D313" s="29">
+        <v>6138883</v>
       </c>
       <c r="E313" s="67" t="s">
         <v>636</v>
@@ -11109,8 +11147,8 @@
       <c r="C314" s="95" t="s">
         <v>629</v>
       </c>
-      <c r="D314" s="29" t="s">
-        <v>630</v>
+      <c r="D314" s="29">
+        <v>6157446</v>
       </c>
       <c r="E314" s="67" t="s">
         <v>631</v>
@@ -11132,8 +11170,8 @@
       <c r="C315" s="95" t="s">
         <v>629</v>
       </c>
-      <c r="D315" s="29" t="s">
-        <v>632</v>
+      <c r="D315" s="29">
+        <v>6157453</v>
       </c>
       <c r="E315" s="67" t="s">
         <v>633</v>
@@ -11153,10 +11191,10 @@
         <v>139</v>
       </c>
       <c r="C316" s="95" t="s">
-        <v>622</v>
-      </c>
-      <c r="D316" s="29" t="s">
-        <v>623</v>
+        <v>832</v>
+      </c>
+      <c r="D316" s="29">
+        <v>6160002</v>
       </c>
       <c r="E316" s="67" t="s">
         <v>624</v>
@@ -11176,10 +11214,10 @@
         <v>139</v>
       </c>
       <c r="C317" s="95" t="s">
-        <v>622</v>
-      </c>
-      <c r="D317" s="29" t="s">
-        <v>625</v>
+        <v>832</v>
+      </c>
+      <c r="D317" s="29">
+        <v>6159988</v>
       </c>
       <c r="E317" s="67" t="s">
         <v>626</v>
@@ -11199,10 +11237,10 @@
         <v>139</v>
       </c>
       <c r="C318" s="95" t="s">
-        <v>622</v>
-      </c>
-      <c r="D318" s="29" t="s">
-        <v>627</v>
+        <v>832</v>
+      </c>
+      <c r="D318" s="29">
+        <v>6159996</v>
       </c>
       <c r="E318" s="67" t="s">
         <v>628</v>
@@ -11216,7 +11254,7 @@
     </row>
     <row r="319" spans="1:7">
       <c r="A319" s="79" t="s">
-        <v>816</v>
+        <v>812</v>
       </c>
       <c r="B319" s="38" t="s">
         <v>388</v>
@@ -11239,13 +11277,13 @@
     </row>
     <row r="320" spans="1:7">
       <c r="A320" s="79" t="s">
-        <v>816</v>
+        <v>812</v>
       </c>
       <c r="B320" s="38" t="s">
         <v>77</v>
       </c>
       <c r="C320" s="61" t="s">
-        <v>391</v>
+        <v>834</v>
       </c>
       <c r="D320" s="28">
         <v>6090209</v>
@@ -11270,8 +11308,8 @@
       <c r="C321" s="61" t="s">
         <v>490</v>
       </c>
-      <c r="D321" s="29" t="s">
-        <v>501</v>
+      <c r="D321" s="29">
+        <v>6241570</v>
       </c>
       <c r="E321" s="67" t="s">
         <v>502</v>
@@ -11293,8 +11331,8 @@
       <c r="C322" s="61" t="s">
         <v>466</v>
       </c>
-      <c r="D322" s="78" t="s">
-        <v>487</v>
+      <c r="D322" s="78">
+        <v>6041368</v>
       </c>
       <c r="E322" s="90" t="s">
         <v>488</v>
@@ -11314,7 +11352,7 @@
         <v>638</v>
       </c>
       <c r="C323" s="61" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="D323" s="36">
         <v>7381475</v>
@@ -11337,7 +11375,7 @@
         <v>8</v>
       </c>
       <c r="C324" s="61" t="s">
-        <v>641</v>
+        <v>825</v>
       </c>
       <c r="D324" s="126">
         <v>7341818</v>
@@ -11360,7 +11398,7 @@
         <v>8</v>
       </c>
       <c r="C325" s="61" t="s">
-        <v>641</v>
+        <v>825</v>
       </c>
       <c r="D325" s="126">
         <v>6022939</v>
@@ -11383,7 +11421,7 @@
         <v>8</v>
       </c>
       <c r="C326" s="61" t="s">
-        <v>641</v>
+        <v>825</v>
       </c>
       <c r="D326" s="126">
         <v>7398628</v>
@@ -11405,8 +11443,8 @@
       <c r="B327" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="C327" s="64" t="s">
-        <v>641</v>
+      <c r="C327" s="61" t="s">
+        <v>825</v>
       </c>
       <c r="D327" s="126">
         <v>6346833</v>
@@ -11428,8 +11466,8 @@
       <c r="B328" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="C328" s="64" t="s">
-        <v>641</v>
+      <c r="C328" s="61" t="s">
+        <v>825</v>
       </c>
       <c r="D328" s="59">
         <v>7065540</v>
@@ -11451,8 +11489,8 @@
       <c r="B329" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="C329" s="64" t="s">
-        <v>641</v>
+      <c r="C329" s="61" t="s">
+        <v>825</v>
       </c>
       <c r="D329" s="59">
         <v>6030189</v>
@@ -11514,13 +11552,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G331" xr:uid="{34D5923A-278D-4369-B8F5-8DD624AEEB26}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G331">
-      <sortCondition ref="A2:A331"/>
-      <sortCondition ref="B2:B331"/>
-      <sortCondition ref="C2:C331"/>
-    </sortState>
-  </autoFilter>
   <phoneticPr fontId="11" type="noConversion"/>
   <conditionalFormatting sqref="E41">
     <cfRule type="expression" dxfId="5" priority="1">
@@ -11534,7 +11565,7 @@
     <cfRule type="duplicateValues" dxfId="3" priority="5"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="50" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" scale="50" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -17402,7 +17433,7 @@
         <v>659</v>
       </c>
       <c r="B6" s="143" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>506</v>
@@ -17417,7 +17448,7 @@
         <v>659</v>
       </c>
       <c r="B7" s="143" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>506</v>
@@ -17522,7 +17553,7 @@
         <v>664</v>
       </c>
       <c r="B14" s="143" t="s">
-        <v>796</v>
+        <v>793</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>34</v>
@@ -17792,7 +17823,7 @@
         <v>672</v>
       </c>
       <c r="B32" s="143" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>79</v>
@@ -17807,7 +17838,7 @@
         <v>672</v>
       </c>
       <c r="B33" s="143" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>79</v>
@@ -17822,7 +17853,7 @@
         <v>672</v>
       </c>
       <c r="B34" s="143" t="s">
-        <v>795</v>
+        <v>792</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>80</v>
@@ -18017,7 +18048,7 @@
         <v>672</v>
       </c>
       <c r="B47" s="143" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
       <c r="C47" s="7" t="s">
         <v>451</v>
@@ -18032,7 +18063,7 @@
         <v>672</v>
       </c>
       <c r="B48" s="143" t="s">
-        <v>798</v>
+        <v>795</v>
       </c>
       <c r="C48" s="7" t="s">
         <v>451</v>
@@ -18047,7 +18078,7 @@
         <v>672</v>
       </c>
       <c r="B49" s="144" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="C49" s="7" t="s">
         <v>451</v>
@@ -18122,7 +18153,7 @@
         <v>672</v>
       </c>
       <c r="B54" s="143" t="s">
-        <v>794</v>
+        <v>791</v>
       </c>
       <c r="C54" s="7" t="s">
         <v>576</v>
@@ -18137,7 +18168,7 @@
         <v>672</v>
       </c>
       <c r="B55" s="143" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="C55" s="7" t="s">
         <v>576</v>
@@ -18152,7 +18183,7 @@
         <v>672</v>
       </c>
       <c r="B56" s="143" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="C56" s="7" t="s">
         <v>576</v>
@@ -18167,7 +18198,7 @@
         <v>672</v>
       </c>
       <c r="B57" s="143" t="s">
-        <v>792</v>
+        <v>789</v>
       </c>
       <c r="C57" s="7" t="s">
         <v>576</v>
@@ -18212,7 +18243,7 @@
         <v>670</v>
       </c>
       <c r="B60" s="143" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="C60" s="7" t="s">
         <v>156</v>
@@ -18227,7 +18258,7 @@
         <v>670</v>
       </c>
       <c r="B61" s="143" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="C61" s="7" t="s">
         <v>156</v>
@@ -18242,7 +18273,7 @@
         <v>670</v>
       </c>
       <c r="B62" s="143" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="C62" s="7" t="s">
         <v>156</v>
@@ -18317,7 +18348,7 @@
         <v>670</v>
       </c>
       <c r="B67" s="144" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="C67" s="7" t="s">
         <v>255</v>
@@ -18332,7 +18363,7 @@
         <v>670</v>
       </c>
       <c r="B68" s="144" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="C68" s="7" t="s">
         <v>266</v>
@@ -18872,7 +18903,7 @@
         <v>676</v>
       </c>
       <c r="B104" s="143" t="s">
-        <v>790</v>
+        <v>787</v>
       </c>
       <c r="C104" s="7" t="s">
         <v>588</v>

</xml_diff>

<commit_message>
Atualizado para o dia 20200514
</commit_message>
<xml_diff>
--- a/obj_2020.xlsx
+++ b/obj_2020.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilizador\PycharmProjects\webcomum\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\users\utilizador\pycharmprojects\webcomum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9E8D9D50-296B-4DF7-99A0-A4124AD6B780}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE309598-8611-44FD-ABD6-201CD97F230D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="15000" xr2:uid="{782B4511-98CD-3642-962C-2459CDADA9BE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{782B4511-98CD-3642-962C-2459CDADA9BE}"/>
   </bookViews>
   <sheets>
     <sheet name="2020" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <definedName name="_FilterDatabase" localSheetId="3" hidden="1">árvore!$A$1:$C$1</definedName>
     <definedName name="_FilterDatabase" localSheetId="2" hidden="1">'CNP Planograma'!$A$1:$E$1</definedName>
     <definedName name="_FilterDatabase" localSheetId="4" hidden="1">inverno!$A$1:$G$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2020'!$A$1:$G$331</definedName>
+    <definedName name="a" localSheetId="0" hidden="1">'2020'!$A$1:$G$331</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -3801,7 +3801,7 @@
   </sheetPr>
   <dimension ref="A1:K331"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
@@ -11713,9 +11713,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30C658BF-D258-4E6D-A4E8-FADEB2BF59DC}">
   <dimension ref="A1:E329"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="14.25"/>
   <cols>
@@ -17321,11 +17319,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E1" xr:uid="{5BF8FF24-7C62-374E-8E65-D92D65D4988C}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E329">
-      <sortCondition ref="A1:A329"/>
-    </sortState>
-  </autoFilter>
   <conditionalFormatting sqref="E39">
     <cfRule type="expression" dxfId="2" priority="1">
       <formula>$E$3="B"</formula>
@@ -17345,8 +17338,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C14684D-4F3A-5E49-A58F-2CA4AA6B0AA1}">
   <dimension ref="A1:D127"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A104" sqref="A104"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75"/>
@@ -21575,18 +21568,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -21793,14 +21786,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8611E8E-EE29-4411-ABA7-B98BAA1AC46E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{746F001C-802F-45DE-9281-826AE8511548}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -21813,6 +21798,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="bcc3b867-df8b-4f81-af6a-0ec368ec18a5"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8611E8E-EE29-4411-ABA7-B98BAA1AC46E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Atualizado para o dia 20200816
</commit_message>
<xml_diff>
--- a/obj_2020.xlsx
+++ b/obj_2020.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\users\utilizador\pycharmprojects\webcomum\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilizador\PycharmProjects\webcomum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE309598-8611-44FD-ABD6-201CD97F230D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F310C861-0C51-4802-9C77-19EFF8BCCF15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{782B4511-98CD-3642-962C-2459CDADA9BE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{782B4511-98CD-3642-962C-2459CDADA9BE}"/>
   </bookViews>
   <sheets>
     <sheet name="2020" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3596" uniqueCount="838">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3596" uniqueCount="837">
   <si>
     <t>Categoria hmR3</t>
   </si>
@@ -2485,9 +2485,6 @@
     <t>Tratamento e cuidado de pernas pesadas sistémico hmR 4</t>
   </si>
   <si>
-    <t>Anti-inflamatórios e Anti-Reumáticos tópicos emplastro hmR 4</t>
-  </si>
-  <si>
     <t>Reguladores da flora intestinal pó hmR 4</t>
   </si>
   <si>
@@ -2498,30 +2495,6 @@
   </si>
   <si>
     <t>Reguladores da flora intestinal comprimidos mastigáveis hmR 4</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Anti-inflamatórios e Anti-Reumáticos tópicos </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Helvetica"/>
-        <family val="2"/>
-      </rPr>
-      <t>SEM EMPLASTROS</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Helvetica"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> hmR 4</t>
-    </r>
   </si>
   <si>
     <r>
@@ -2621,6 +2594,21 @@
   </si>
   <si>
     <t>Pedisilk</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Anti-inflamatórios e Anti-Reumáticos tópicos </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>SEM EMPLASTROS</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2950,7 +2938,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="155">
+  <cellXfs count="154">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3357,9 +3345,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3801,8 +3786,8 @@
   </sheetPr>
   <dimension ref="A1:K331"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A71" sqref="A71:A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="14.25"/>
@@ -3838,7 +3823,7 @@
       <c r="F1" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="153" t="s">
+      <c r="G1" s="152" t="s">
         <v>6</v>
       </c>
     </row>
@@ -4355,7 +4340,7 @@
         <v>13</v>
       </c>
       <c r="C23" s="60" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="D23" s="28">
         <v>6226506</v>
@@ -4379,7 +4364,7 @@
         <v>13</v>
       </c>
       <c r="C24" s="60" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="D24" s="28">
         <v>6406413</v>
@@ -4907,7 +4892,7 @@
         <v>8</v>
       </c>
       <c r="C46" s="60" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="D46" s="29">
         <v>6004424</v>
@@ -5083,7 +5068,7 @@
       <c r="E53" s="66" t="s">
         <v>157</v>
       </c>
-      <c r="F53" s="151">
+      <c r="F53" s="150">
         <v>0.38</v>
       </c>
       <c r="G53" s="83">
@@ -5107,7 +5092,7 @@
       <c r="E54" s="66" t="s">
         <v>159</v>
       </c>
-      <c r="F54" s="151">
+      <c r="F54" s="150">
         <v>0.25</v>
       </c>
       <c r="G54" s="83">
@@ -5131,7 +5116,7 @@
       <c r="E55" s="66" t="s">
         <v>155</v>
       </c>
-      <c r="F55" s="151">
+      <c r="F55" s="150">
         <v>1</v>
       </c>
       <c r="G55" s="83">
@@ -5155,7 +5140,7 @@
       <c r="E56" s="66" t="s">
         <v>160</v>
       </c>
-      <c r="F56" s="151">
+      <c r="F56" s="150">
         <v>0.3</v>
       </c>
       <c r="G56" s="83">
@@ -5195,7 +5180,7 @@
         <v>90</v>
       </c>
       <c r="C58" s="65" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="D58" s="28">
         <v>5337498</v>
@@ -5243,7 +5228,7 @@
         <v>55</v>
       </c>
       <c r="C60" s="65" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="D60" s="28">
         <v>8573014</v>
@@ -5267,7 +5252,7 @@
         <v>13</v>
       </c>
       <c r="C61" s="65" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="D61" s="28">
         <v>6968438</v>
@@ -5315,7 +5300,7 @@
         <v>55</v>
       </c>
       <c r="C63" s="65" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="D63" s="28">
         <v>8289611</v>
@@ -5501,7 +5486,7 @@
     </row>
     <row r="71" spans="1:10" ht="15.95" customHeight="1">
       <c r="A71" s="80" t="s">
-        <v>813</v>
+        <v>746</v>
       </c>
       <c r="B71" s="22" t="s">
         <v>28</v>
@@ -5525,7 +5510,7 @@
     </row>
     <row r="72" spans="1:10">
       <c r="A72" s="80" t="s">
-        <v>813</v>
+        <v>746</v>
       </c>
       <c r="B72" s="38" t="s">
         <v>139</v>
@@ -5549,7 +5534,7 @@
     </row>
     <row r="73" spans="1:10" ht="15.95" customHeight="1">
       <c r="A73" s="80" t="s">
-        <v>818</v>
+        <v>836</v>
       </c>
       <c r="B73" s="22" t="s">
         <v>749</v>
@@ -5573,7 +5558,7 @@
     </row>
     <row r="74" spans="1:10" ht="15">
       <c r="A74" s="80" t="s">
-        <v>818</v>
+        <v>836</v>
       </c>
       <c r="B74" s="38" t="s">
         <v>749</v>
@@ -5596,8 +5581,8 @@
       <c r="J74" s="51"/>
     </row>
     <row r="75" spans="1:10" ht="15.95" customHeight="1">
-      <c r="A75" s="138" t="s">
-        <v>818</v>
+      <c r="A75" s="80" t="s">
+        <v>836</v>
       </c>
       <c r="B75" s="32" t="s">
         <v>749</v>
@@ -5620,8 +5605,8 @@
       <c r="J75" s="51"/>
     </row>
     <row r="76" spans="1:10" ht="15.95" customHeight="1">
-      <c r="A76" s="138" t="s">
-        <v>818</v>
+      <c r="A76" s="80" t="s">
+        <v>836</v>
       </c>
       <c r="B76" s="22" t="s">
         <v>749</v>
@@ -5645,7 +5630,7 @@
     </row>
     <row r="77" spans="1:10" ht="15.95" customHeight="1">
       <c r="A77" s="80" t="s">
-        <v>818</v>
+        <v>836</v>
       </c>
       <c r="B77" s="22" t="s">
         <v>749</v>
@@ -5669,7 +5654,7 @@
     </row>
     <row r="78" spans="1:10" ht="15">
       <c r="A78" s="80" t="s">
-        <v>818</v>
+        <v>836</v>
       </c>
       <c r="B78" s="38" t="s">
         <v>749</v>
@@ -5693,13 +5678,13 @@
     </row>
     <row r="79" spans="1:10" ht="15.95" customHeight="1">
       <c r="A79" s="80" t="s">
-        <v>818</v>
+        <v>836</v>
       </c>
       <c r="B79" s="22" t="s">
         <v>28</v>
       </c>
       <c r="C79" s="60" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="D79" s="28">
         <v>5197868</v>
@@ -5717,13 +5702,13 @@
     </row>
     <row r="80" spans="1:10" ht="15.95" customHeight="1">
       <c r="A80" s="80" t="s">
-        <v>818</v>
+        <v>836</v>
       </c>
       <c r="B80" s="22" t="s">
         <v>28</v>
       </c>
       <c r="C80" s="60" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="D80" s="28">
         <v>5035654</v>
@@ -5741,13 +5726,13 @@
     </row>
     <row r="81" spans="1:10" ht="15">
       <c r="A81" s="80" t="s">
-        <v>818</v>
+        <v>836</v>
       </c>
       <c r="B81" s="38" t="s">
         <v>28</v>
       </c>
       <c r="C81" s="60" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="D81" s="28">
         <v>5712740</v>
@@ -5765,13 +5750,13 @@
     </row>
     <row r="82" spans="1:10" ht="15">
       <c r="A82" s="80" t="s">
-        <v>818</v>
+        <v>836</v>
       </c>
       <c r="B82" s="22" t="s">
         <v>28</v>
       </c>
       <c r="C82" s="60" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="D82" s="28">
         <v>5219316</v>
@@ -5789,15 +5774,15 @@
     </row>
     <row r="83" spans="1:10" ht="15">
       <c r="A83" s="80" t="s">
-        <v>818</v>
+        <v>836</v>
       </c>
       <c r="B83" s="22" t="s">
         <v>28</v>
       </c>
       <c r="C83" s="60" t="s">
-        <v>824</v>
-      </c>
-      <c r="D83" s="154">
+        <v>822</v>
+      </c>
+      <c r="D83" s="153">
         <v>5374848</v>
       </c>
       <c r="E83" s="100" t="s">
@@ -5813,13 +5798,13 @@
     </row>
     <row r="84" spans="1:10" ht="15">
       <c r="A84" s="80" t="s">
-        <v>818</v>
+        <v>836</v>
       </c>
       <c r="B84" s="22" t="s">
         <v>28</v>
       </c>
       <c r="C84" s="60" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="D84" s="28">
         <v>5625025</v>
@@ -5837,13 +5822,13 @@
     </row>
     <row r="85" spans="1:10" ht="15">
       <c r="A85" s="80" t="s">
-        <v>818</v>
+        <v>836</v>
       </c>
       <c r="B85" s="22" t="s">
         <v>28</v>
       </c>
       <c r="C85" s="60" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="D85" s="102">
         <v>5380571</v>
@@ -6035,7 +6020,7 @@
         <v>24</v>
       </c>
       <c r="C93" s="60" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="D93" s="29">
         <v>6317586</v>
@@ -6059,7 +6044,7 @@
         <v>24</v>
       </c>
       <c r="C94" s="60" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="D94" s="29">
         <v>6942466</v>
@@ -6083,7 +6068,7 @@
         <v>24</v>
       </c>
       <c r="C95" s="60" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="D95" s="29">
         <v>7008029</v>
@@ -6107,7 +6092,7 @@
         <v>24</v>
       </c>
       <c r="C96" s="60" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="D96" s="29">
         <v>6992040</v>
@@ -6131,7 +6116,7 @@
         <v>24</v>
       </c>
       <c r="C97" s="60" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="D97" s="29">
         <v>7471698</v>
@@ -6155,7 +6140,7 @@
         <v>24</v>
       </c>
       <c r="C98" s="60" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="D98" s="29">
         <v>6076588</v>
@@ -6331,7 +6316,7 @@
       <c r="E105" s="112" t="s">
         <v>170</v>
       </c>
-      <c r="F105" s="150">
+      <c r="F105" s="149">
         <v>0.04</v>
       </c>
       <c r="G105" s="117">
@@ -6523,7 +6508,7 @@
       <c r="E113" s="67" t="s">
         <v>194</v>
       </c>
-      <c r="F113" s="140">
+      <c r="F113" s="139">
         <v>0.05</v>
       </c>
       <c r="G113" s="83">
@@ -7419,7 +7404,7 @@
         <v>8</v>
       </c>
       <c r="C152" s="60" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="D152" s="44">
         <v>9908756</v>
@@ -7442,7 +7427,7 @@
         <v>8</v>
       </c>
       <c r="C153" s="60" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="D153" s="44">
         <v>9908731</v>
@@ -7597,7 +7582,7 @@
     </row>
     <row r="160" spans="1:7" ht="15.95" customHeight="1">
       <c r="A160" s="72" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="B160" s="22" t="s">
         <v>139</v>
@@ -7611,7 +7596,7 @@
       <c r="E160" s="66" t="s">
         <v>462</v>
       </c>
-      <c r="F160" s="149">
+      <c r="F160" s="148">
         <v>0.65</v>
       </c>
       <c r="G160" s="131">
@@ -7620,7 +7605,7 @@
     </row>
     <row r="161" spans="1:7" ht="15.95" customHeight="1">
       <c r="A161" s="72" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="B161" s="22" t="s">
         <v>139</v>
@@ -7634,7 +7619,7 @@
       <c r="E161" s="66" t="s">
         <v>464</v>
       </c>
-      <c r="F161" s="149">
+      <c r="F161" s="148">
         <v>0.65</v>
       </c>
       <c r="G161" s="131">
@@ -7766,7 +7751,7 @@
       <c r="C167" s="64" t="s">
         <v>293</v>
       </c>
-      <c r="D167" s="148">
+      <c r="D167" s="147">
         <v>5633326</v>
       </c>
       <c r="E167" s="67" t="s">
@@ -7902,7 +7887,7 @@
         <v>403</v>
       </c>
       <c r="C173" s="65" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="D173" s="28">
         <v>6097147</v>
@@ -7948,7 +7933,7 @@
         <v>403</v>
       </c>
       <c r="C175" s="65" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="D175" s="28">
         <v>6097154</v>
@@ -7971,7 +7956,7 @@
         <v>403</v>
       </c>
       <c r="C176" s="65" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="D176" s="28">
         <v>6097162</v>
@@ -8071,7 +8056,7 @@
       <c r="E180" s="119" t="s">
         <v>307</v>
       </c>
-      <c r="F180" s="152">
+      <c r="F180" s="151">
         <v>0.5</v>
       </c>
       <c r="G180" s="117">
@@ -8094,7 +8079,7 @@
       <c r="E181" s="119" t="s">
         <v>309</v>
       </c>
-      <c r="F181" s="152">
+      <c r="F181" s="151">
         <v>0.03</v>
       </c>
       <c r="G181" s="117">
@@ -8453,7 +8438,7 @@
       <c r="B197" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="C197" s="146" t="s">
+      <c r="C197" s="145" t="s">
         <v>311</v>
       </c>
       <c r="D197" s="104">
@@ -8804,7 +8789,7 @@
       <c r="D212" s="28">
         <v>5154778</v>
       </c>
-      <c r="E212" s="139" t="s">
+      <c r="E212" s="138" t="s">
         <v>429</v>
       </c>
       <c r="F212" s="85">
@@ -9057,7 +9042,7 @@
       <c r="D223" s="44">
         <v>5744370</v>
       </c>
-      <c r="E223" s="142" t="s">
+      <c r="E223" s="141" t="s">
         <v>420</v>
       </c>
       <c r="F223" s="77">
@@ -9092,7 +9077,7 @@
     </row>
     <row r="225" spans="1:7" ht="15">
       <c r="A225" s="72" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="B225" s="22" t="s">
         <v>748</v>
@@ -9115,7 +9100,7 @@
     </row>
     <row r="226" spans="1:7" ht="15">
       <c r="A226" s="72" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="B226" s="22" t="s">
         <v>28</v>
@@ -9138,7 +9123,7 @@
     </row>
     <row r="227" spans="1:7" ht="15">
       <c r="A227" s="72" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="B227" s="22" t="s">
         <v>13</v>
@@ -9161,7 +9146,7 @@
     </row>
     <row r="228" spans="1:7" ht="15">
       <c r="A228" s="72" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="B228" s="22" t="s">
         <v>450</v>
@@ -9184,7 +9169,7 @@
     </row>
     <row r="229" spans="1:7" ht="15">
       <c r="A229" s="72" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="B229" s="22" t="s">
         <v>450</v>
@@ -9207,7 +9192,7 @@
     </row>
     <row r="230" spans="1:7" ht="15">
       <c r="A230" s="72" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="B230" s="22" t="s">
         <v>450</v>
@@ -9230,7 +9215,7 @@
     </row>
     <row r="231" spans="1:7" ht="15">
       <c r="A231" s="72" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="B231" s="22" t="s">
         <v>450</v>
@@ -9253,7 +9238,7 @@
     </row>
     <row r="232" spans="1:7" ht="15">
       <c r="A232" s="72" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="B232" s="38" t="s">
         <v>450</v>
@@ -9276,7 +9261,7 @@
     </row>
     <row r="233" spans="1:7" ht="15">
       <c r="A233" s="72" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="B233" s="43" t="s">
         <v>139</v>
@@ -10449,13 +10434,13 @@
     </row>
     <row r="284" spans="1:7">
       <c r="A284" s="80" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="B284" s="22" t="s">
         <v>28</v>
       </c>
       <c r="C284" s="65" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="D284" s="28">
         <v>6284885</v>
@@ -10472,13 +10457,13 @@
     </row>
     <row r="285" spans="1:7">
       <c r="A285" s="80" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="B285" s="22" t="s">
         <v>28</v>
       </c>
       <c r="C285" s="65" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="D285" s="28">
         <v>6334722</v>
@@ -10495,13 +10480,13 @@
     </row>
     <row r="286" spans="1:7">
       <c r="A286" s="80" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="B286" s="22" t="s">
         <v>371</v>
       </c>
       <c r="C286" s="65" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="D286" s="28">
         <v>6180554</v>
@@ -10518,13 +10503,13 @@
     </row>
     <row r="287" spans="1:7">
       <c r="A287" s="80" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="B287" s="22" t="s">
         <v>371</v>
       </c>
       <c r="C287" s="65" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="D287" s="28">
         <v>6294736</v>
@@ -10541,13 +10526,13 @@
     </row>
     <row r="288" spans="1:7">
       <c r="A288" s="80" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="B288" s="22" t="s">
         <v>371</v>
       </c>
       <c r="C288" s="65" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="D288" s="28">
         <v>6294744</v>
@@ -10564,13 +10549,13 @@
     </row>
     <row r="289" spans="1:7">
       <c r="A289" s="80" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="B289" s="22" t="s">
         <v>371</v>
       </c>
       <c r="C289" s="65" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="D289" s="28">
         <v>6180562</v>
@@ -10587,13 +10572,13 @@
     </row>
     <row r="290" spans="1:7">
       <c r="A290" s="80" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="B290" s="22" t="s">
         <v>371</v>
       </c>
       <c r="C290" s="65" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="D290" s="28">
         <v>6317792</v>
@@ -10610,13 +10595,13 @@
     </row>
     <row r="291" spans="1:7">
       <c r="A291" s="72" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="B291" s="22" t="s">
         <v>73</v>
       </c>
       <c r="C291" s="65" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="D291" s="28">
         <v>6349068</v>
@@ -10633,7 +10618,7 @@
     </row>
     <row r="292" spans="1:7">
       <c r="A292" s="72" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="B292" s="22" t="s">
         <v>139</v>
@@ -10656,7 +10641,7 @@
     </row>
     <row r="293" spans="1:7">
       <c r="A293" s="72" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="B293" s="22" t="s">
         <v>139</v>
@@ -10679,7 +10664,7 @@
     </row>
     <row r="294" spans="1:7">
       <c r="A294" s="72" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="B294" s="22" t="s">
         <v>579</v>
@@ -10702,7 +10687,7 @@
     </row>
     <row r="295" spans="1:7">
       <c r="A295" s="72" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="B295" s="22" t="s">
         <v>579</v>
@@ -10750,7 +10735,7 @@
       <c r="A297" s="72" t="s">
         <v>587</v>
       </c>
-      <c r="B297" s="145" t="s">
+      <c r="B297" s="144" t="s">
         <v>18</v>
       </c>
       <c r="C297" s="124" t="s">
@@ -10773,7 +10758,7 @@
       <c r="A298" s="72" t="s">
         <v>787</v>
       </c>
-      <c r="B298" s="145" t="s">
+      <c r="B298" s="144" t="s">
         <v>732</v>
       </c>
       <c r="C298" s="124" t="s">
@@ -10868,7 +10853,7 @@
       <c r="B302" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="C302" s="147" t="s">
+      <c r="C302" s="146" t="s">
         <v>667</v>
       </c>
       <c r="D302" s="29">
@@ -10891,7 +10876,7 @@
       <c r="B303" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="C303" s="147" t="s">
+      <c r="C303" s="146" t="s">
         <v>667</v>
       </c>
       <c r="D303" s="29">
@@ -10914,7 +10899,7 @@
       <c r="B304" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="C304" s="147" t="s">
+      <c r="C304" s="146" t="s">
         <v>667</v>
       </c>
       <c r="D304" s="29">
@@ -10937,7 +10922,7 @@
       <c r="B305" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="C305" s="147" t="s">
+      <c r="C305" s="146" t="s">
         <v>667</v>
       </c>
       <c r="D305" s="29">
@@ -10960,7 +10945,7 @@
       <c r="B306" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="C306" s="147" t="s">
+      <c r="C306" s="146" t="s">
         <v>667</v>
       </c>
       <c r="D306" s="29">
@@ -10983,7 +10968,7 @@
       <c r="B307" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="C307" s="147" t="s">
+      <c r="C307" s="146" t="s">
         <v>667</v>
       </c>
       <c r="D307" s="28">
@@ -11006,7 +10991,7 @@
       <c r="B308" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="C308" s="147" t="s">
+      <c r="C308" s="146" t="s">
         <v>667</v>
       </c>
       <c r="D308" s="28">
@@ -11029,7 +11014,7 @@
       <c r="B309" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="C309" s="147" t="s">
+      <c r="C309" s="146" t="s">
         <v>667</v>
       </c>
       <c r="D309" s="74">
@@ -11052,7 +11037,7 @@
       <c r="B310" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="C310" s="147" t="s">
+      <c r="C310" s="146" t="s">
         <v>667</v>
       </c>
       <c r="D310" s="28">
@@ -11075,7 +11060,7 @@
       <c r="B311" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="C311" s="147" t="s">
+      <c r="C311" s="146" t="s">
         <v>667</v>
       </c>
       <c r="D311" s="28">
@@ -11098,7 +11083,7 @@
       <c r="B312" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="C312" s="147" t="s">
+      <c r="C312" s="146" t="s">
         <v>667</v>
       </c>
       <c r="D312" s="28">
@@ -11191,7 +11176,7 @@
         <v>139</v>
       </c>
       <c r="C316" s="95" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="D316" s="29">
         <v>6160002</v>
@@ -11214,7 +11199,7 @@
         <v>139</v>
       </c>
       <c r="C317" s="95" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="D317" s="29">
         <v>6159988</v>
@@ -11237,7 +11222,7 @@
         <v>139</v>
       </c>
       <c r="C318" s="95" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="D318" s="29">
         <v>6159996</v>
@@ -11283,7 +11268,7 @@
         <v>77</v>
       </c>
       <c r="C320" s="61" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="D320" s="28">
         <v>6090209</v>
@@ -11375,7 +11360,7 @@
         <v>8</v>
       </c>
       <c r="C324" s="61" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="D324" s="126">
         <v>7341818</v>
@@ -11398,7 +11383,7 @@
         <v>8</v>
       </c>
       <c r="C325" s="61" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="D325" s="126">
         <v>6022939</v>
@@ -11421,7 +11406,7 @@
         <v>8</v>
       </c>
       <c r="C326" s="61" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="D326" s="126">
         <v>7398628</v>
@@ -11444,7 +11429,7 @@
         <v>8</v>
       </c>
       <c r="C327" s="61" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="D327" s="126">
         <v>6346833</v>
@@ -11467,7 +11452,7 @@
         <v>8</v>
       </c>
       <c r="C328" s="61" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="D328" s="59">
         <v>7065540</v>
@@ -11490,7 +11475,7 @@
         <v>8</v>
       </c>
       <c r="C329" s="61" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="D329" s="59">
         <v>6030189</v>
@@ -11580,7 +11565,7 @@
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="24.125" style="52" customWidth="1"/>
-    <col min="2" max="16384" width="10.875" style="141"/>
+    <col min="2" max="16384" width="10.875" style="140"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -17338,7 +17323,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C14684D-4F3A-5E49-A58F-2CA4AA6B0AA1}">
   <dimension ref="A1:D127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
@@ -17425,7 +17410,7 @@
       <c r="A6" s="4" t="s">
         <v>659</v>
       </c>
-      <c r="B6" s="143" t="s">
+      <c r="B6" s="142" t="s">
         <v>771</v>
       </c>
       <c r="C6" s="7" t="s">
@@ -17440,7 +17425,7 @@
       <c r="A7" s="4" t="s">
         <v>659</v>
       </c>
-      <c r="B7" s="143" t="s">
+      <c r="B7" s="142" t="s">
         <v>772</v>
       </c>
       <c r="C7" s="7" t="s">
@@ -17455,7 +17440,7 @@
       <c r="A8" s="4" t="s">
         <v>659</v>
       </c>
-      <c r="B8" s="143" t="s">
+      <c r="B8" s="142" t="s">
         <v>505</v>
       </c>
       <c r="C8" s="7" t="s">
@@ -17545,7 +17530,7 @@
       <c r="A14" s="91" t="s">
         <v>664</v>
       </c>
-      <c r="B14" s="143" t="s">
+      <c r="B14" s="142" t="s">
         <v>793</v>
       </c>
       <c r="C14" s="5" t="s">
@@ -17695,7 +17680,7 @@
       <c r="A24" s="91" t="s">
         <v>664</v>
       </c>
-      <c r="B24" s="143" t="s">
+      <c r="B24" s="142" t="s">
         <v>723</v>
       </c>
       <c r="C24" s="7" t="s">
@@ -17815,7 +17800,7 @@
       <c r="A32" s="4" t="s">
         <v>672</v>
       </c>
-      <c r="B32" s="143" t="s">
+      <c r="B32" s="142" t="s">
         <v>778</v>
       </c>
       <c r="C32" s="7" t="s">
@@ -17830,7 +17815,7 @@
       <c r="A33" s="4" t="s">
         <v>672</v>
       </c>
-      <c r="B33" s="143" t="s">
+      <c r="B33" s="142" t="s">
         <v>777</v>
       </c>
       <c r="C33" s="7" t="s">
@@ -17845,7 +17830,7 @@
       <c r="A34" s="4" t="s">
         <v>672</v>
       </c>
-      <c r="B34" s="143" t="s">
+      <c r="B34" s="142" t="s">
         <v>792</v>
       </c>
       <c r="C34" s="7" t="s">
@@ -18040,7 +18025,7 @@
       <c r="A47" s="4" t="s">
         <v>672</v>
       </c>
-      <c r="B47" s="143" t="s">
+      <c r="B47" s="142" t="s">
         <v>794</v>
       </c>
       <c r="C47" s="7" t="s">
@@ -18055,7 +18040,7 @@
       <c r="A48" s="4" t="s">
         <v>672</v>
       </c>
-      <c r="B48" s="143" t="s">
+      <c r="B48" s="142" t="s">
         <v>795</v>
       </c>
       <c r="C48" s="7" t="s">
@@ -18070,7 +18055,7 @@
       <c r="A49" s="4" t="s">
         <v>672</v>
       </c>
-      <c r="B49" s="144" t="s">
+      <c r="B49" s="143" t="s">
         <v>782</v>
       </c>
       <c r="C49" s="7" t="s">
@@ -18145,7 +18130,7 @@
       <c r="A54" s="4" t="s">
         <v>672</v>
       </c>
-      <c r="B54" s="143" t="s">
+      <c r="B54" s="142" t="s">
         <v>791</v>
       </c>
       <c r="C54" s="7" t="s">
@@ -18160,7 +18145,7 @@
       <c r="A55" s="4" t="s">
         <v>672</v>
       </c>
-      <c r="B55" s="143" t="s">
+      <c r="B55" s="142" t="s">
         <v>790</v>
       </c>
       <c r="C55" s="7" t="s">
@@ -18175,7 +18160,7 @@
       <c r="A56" s="4" t="s">
         <v>672</v>
       </c>
-      <c r="B56" s="143" t="s">
+      <c r="B56" s="142" t="s">
         <v>788</v>
       </c>
       <c r="C56" s="7" t="s">
@@ -18190,7 +18175,7 @@
       <c r="A57" s="4" t="s">
         <v>672</v>
       </c>
-      <c r="B57" s="143" t="s">
+      <c r="B57" s="142" t="s">
         <v>789</v>
       </c>
       <c r="C57" s="7" t="s">
@@ -18235,7 +18220,7 @@
       <c r="A60" s="4" t="s">
         <v>670</v>
       </c>
-      <c r="B60" s="143" t="s">
+      <c r="B60" s="142" t="s">
         <v>779</v>
       </c>
       <c r="C60" s="7" t="s">
@@ -18250,7 +18235,7 @@
       <c r="A61" s="4" t="s">
         <v>670</v>
       </c>
-      <c r="B61" s="143" t="s">
+      <c r="B61" s="142" t="s">
         <v>781</v>
       </c>
       <c r="C61" s="7" t="s">
@@ -18265,7 +18250,7 @@
       <c r="A62" s="4" t="s">
         <v>670</v>
       </c>
-      <c r="B62" s="143" t="s">
+      <c r="B62" s="142" t="s">
         <v>780</v>
       </c>
       <c r="C62" s="7" t="s">
@@ -18340,7 +18325,7 @@
       <c r="A67" s="4" t="s">
         <v>670</v>
       </c>
-      <c r="B67" s="144" t="s">
+      <c r="B67" s="143" t="s">
         <v>783</v>
       </c>
       <c r="C67" s="7" t="s">
@@ -18355,7 +18340,7 @@
       <c r="A68" s="4" t="s">
         <v>670</v>
       </c>
-      <c r="B68" s="144" t="s">
+      <c r="B68" s="143" t="s">
         <v>784</v>
       </c>
       <c r="C68" s="7" t="s">
@@ -18895,7 +18880,7 @@
       <c r="A104" s="4" t="s">
         <v>676</v>
       </c>
-      <c r="B104" s="143" t="s">
+      <c r="B104" s="142" t="s">
         <v>787</v>
       </c>
       <c r="C104" s="7" t="s">
@@ -21568,21 +21553,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D97AAC6AADCCB34E981EC65B77E00DC2" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d92f6cb7e2cbcb2f99017ea5c5e8c1a7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="39513749-c621-4356-ae9e-575f9f637b2c" xmlns:ns3="bcc3b867-df8b-4f81-af6a-0ec368ec18a5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="06a8b1dd7ce196a50e2316c70a2eb4d0" ns2:_="" ns3:_="">
     <xsd:import namespace="39513749-c621-4356-ae9e-575f9f637b2c"/>
@@ -21785,32 +21755,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{746F001C-802F-45DE-9281-826AE8511548}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="39513749-c621-4356-ae9e-575f9f637b2c"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="bcc3b867-df8b-4f81-af6a-0ec368ec18a5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8611E8E-EE29-4411-ABA7-B98BAA1AC46E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57460E9B-3170-4EA4-81EF-FF4925ABB195}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -21827,4 +21787,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8611E8E-EE29-4411-ABA7-B98BAA1AC46E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{746F001C-802F-45DE-9281-826AE8511548}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="39513749-c621-4356-ae9e-575f9f637b2c"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="bcc3b867-df8b-4f81-af6a-0ec368ec18a5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>